<commit_message>
feat:se implementa el conteo de los 60 dias para la precipitacion y la radiacion
</commit_message>
<xml_diff>
--- a/resumen_semanal_clima.xlsx
+++ b/resumen_semanal_clima.xlsx
@@ -511,7 +511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O155"/>
+  <dimension ref="A1:Q155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,15 +582,25 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>Precipitación estimada acumulada últimos 60 días (mm)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Radiación estimada acumulada últimos 60 días (Wh/m²)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>HDD acumulado últimos 60 días</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Días con heladas (&lt; 4 °C)</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Días soleados (Solar &gt; 0 W/m²)</t>
         </is>
@@ -634,12 +644,18 @@
         <v>515.775</v>
       </c>
       <c r="M2" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="N2" t="n">
+        <v>19635.5</v>
+      </c>
+      <c r="O2" t="n">
         <v>515.775</v>
       </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
         <v>7</v>
       </c>
     </row>
@@ -681,12 +697,18 @@
         <v>587.325</v>
       </c>
       <c r="M3" t="n">
+        <v>49.3</v>
+      </c>
+      <c r="N3" t="n">
+        <v>41539.5</v>
+      </c>
+      <c r="O3" t="n">
         <v>1103.1</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>7</v>
       </c>
     </row>
@@ -728,12 +750,18 @@
         <v>555.525</v>
       </c>
       <c r="M4" t="n">
+        <v>77.55</v>
+      </c>
+      <c r="N4" t="n">
+        <v>62166.75</v>
+      </c>
+      <c r="O4" t="n">
         <v>1658.625</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
         <v>7</v>
       </c>
     </row>
@@ -775,12 +803,18 @@
         <v>511.45</v>
       </c>
       <c r="M5" t="n">
+        <v>113.6</v>
+      </c>
+      <c r="N5" t="n">
+        <v>85339.25</v>
+      </c>
+      <c r="O5" t="n">
         <v>2170.075</v>
       </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
         <v>7</v>
       </c>
     </row>
@@ -822,12 +856,18 @@
         <v>533.5</v>
       </c>
       <c r="M6" t="n">
+        <v>127</v>
+      </c>
+      <c r="N6" t="n">
+        <v>114518.5</v>
+      </c>
+      <c r="O6" t="n">
         <v>2703.575</v>
       </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
         <v>7</v>
       </c>
     </row>
@@ -869,12 +909,18 @@
         <v>458.15</v>
       </c>
       <c r="M7" t="n">
+        <v>139.875</v>
+      </c>
+      <c r="N7" t="n">
+        <v>138319.75</v>
+      </c>
+      <c r="O7" t="n">
         <v>3161.725</v>
       </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
         <v>7</v>
       </c>
     </row>
@@ -916,12 +962,18 @@
         <v>539.025</v>
       </c>
       <c r="M8" t="n">
+        <v>158.875</v>
+      </c>
+      <c r="N8" t="n">
+        <v>159717</v>
+      </c>
+      <c r="O8" t="n">
         <v>3700.75</v>
       </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
         <v>7</v>
       </c>
     </row>
@@ -963,12 +1015,18 @@
         <v>523.05</v>
       </c>
       <c r="M9" t="n">
+        <v>158.875</v>
+      </c>
+      <c r="N9" t="n">
+        <v>183103.25</v>
+      </c>
+      <c r="O9" t="n">
         <v>4223.8</v>
       </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1010,12 +1068,18 @@
         <v>515.5</v>
       </c>
       <c r="M10" t="n">
+        <v>174.75</v>
+      </c>
+      <c r="N10" t="n">
+        <v>198683.75</v>
+      </c>
+      <c r="O10" t="n">
         <v>4223.525</v>
       </c>
-      <c r="N10" t="n">
+      <c r="P10" t="n">
         <v>1</v>
       </c>
-      <c r="O10" t="n">
+      <c r="Q10" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1057,12 +1121,18 @@
         <v>461.7</v>
       </c>
       <c r="M11" t="n">
+        <v>196.7</v>
+      </c>
+      <c r="N11" t="n">
+        <v>203377.5</v>
+      </c>
+      <c r="O11" t="n">
         <v>4097.9</v>
       </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1104,12 +1174,18 @@
         <v>565.275</v>
       </c>
       <c r="M12" t="n">
+        <v>189.125</v>
+      </c>
+      <c r="N12" t="n">
+        <v>208308</v>
+      </c>
+      <c r="O12" t="n">
         <v>4107.65</v>
       </c>
-      <c r="N12" t="n">
+      <c r="P12" t="n">
         <v>1</v>
       </c>
-      <c r="O12" t="n">
+      <c r="Q12" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1151,12 +1227,18 @@
         <v>546.3</v>
       </c>
       <c r="M13" t="n">
+        <v>201.75</v>
+      </c>
+      <c r="N13" t="n">
+        <v>209152</v>
+      </c>
+      <c r="O13" t="n">
         <v>4142.5</v>
       </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="n">
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1198,12 +1280,18 @@
         <v>80.3</v>
       </c>
       <c r="M14" t="n">
+        <v>201.75</v>
+      </c>
+      <c r="N14" t="n">
+        <v>209322.75</v>
+      </c>
+      <c r="O14" t="n">
         <v>3689.3</v>
       </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1245,12 +1333,18 @@
         <v>330.775</v>
       </c>
       <c r="M15" t="n">
+        <v>182.35</v>
+      </c>
+      <c r="N15" t="n">
+        <v>207287.25</v>
+      </c>
+      <c r="O15" t="n">
         <v>3561.925</v>
       </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1292,12 +1386,18 @@
         <v>514.575</v>
       </c>
       <c r="M16" t="n">
+        <v>194.65</v>
+      </c>
+      <c r="N16" t="n">
+        <v>199776.5</v>
+      </c>
+      <c r="O16" t="n">
         <v>3537.475</v>
       </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="n">
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1339,12 +1439,18 @@
         <v>561.7</v>
       </c>
       <c r="M17" t="n">
+        <v>194.075</v>
+      </c>
+      <c r="N17" t="n">
+        <v>201090.25</v>
+      </c>
+      <c r="O17" t="n">
         <v>3576.125</v>
       </c>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" t="n">
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1386,12 +1492,18 @@
         <v>619.4</v>
       </c>
       <c r="M18" t="n">
+        <v>201.125</v>
+      </c>
+      <c r="N18" t="n">
+        <v>203279.75</v>
+      </c>
+      <c r="O18" t="n">
         <v>3680.025</v>
       </c>
-      <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="n">
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1433,12 +1545,18 @@
         <v>687.45</v>
       </c>
       <c r="M19" t="n">
+        <v>229.025</v>
+      </c>
+      <c r="N19" t="n">
+        <v>203041.5</v>
+      </c>
+      <c r="O19" t="n">
         <v>3905.775</v>
       </c>
-      <c r="N19" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" t="n">
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1480,12 +1598,18 @@
         <v>605.575</v>
       </c>
       <c r="M20" t="n">
+        <v>202.975</v>
+      </c>
+      <c r="N20" t="n">
+        <v>205814.5</v>
+      </c>
+      <c r="O20" t="n">
         <v>3946.075</v>
       </c>
-      <c r="N20" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" t="n">
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1527,12 +1651,18 @@
         <v>549.975</v>
       </c>
       <c r="M21" t="n">
+        <v>183.65</v>
+      </c>
+      <c r="N21" t="n">
+        <v>208282.75</v>
+      </c>
+      <c r="O21" t="n">
         <v>3949.75</v>
       </c>
-      <c r="N21" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" t="n">
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1574,12 +1704,18 @@
         <v>523.775</v>
       </c>
       <c r="M22" t="n">
+        <v>164.95</v>
+      </c>
+      <c r="N22" t="n">
+        <v>203516.75</v>
+      </c>
+      <c r="O22" t="n">
         <v>4393.225</v>
       </c>
-      <c r="N22" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" t="n">
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1621,12 +1757,18 @@
         <v>391.475</v>
       </c>
       <c r="M23" t="n">
+        <v>152.375</v>
+      </c>
+      <c r="N23" t="n">
+        <v>205647.75</v>
+      </c>
+      <c r="O23" t="n">
         <v>4453.925</v>
       </c>
-      <c r="N23" t="n">
+      <c r="P23" t="n">
         <v>2</v>
       </c>
-      <c r="O23" t="n">
+      <c r="Q23" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1668,12 +1810,18 @@
         <v>537.125</v>
       </c>
       <c r="M24" t="n">
+        <v>128.775</v>
+      </c>
+      <c r="N24" t="n">
+        <v>224838.5</v>
+      </c>
+      <c r="O24" t="n">
         <v>4476.475</v>
       </c>
-      <c r="N24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" t="n">
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1715,12 +1863,18 @@
         <v>546.525</v>
       </c>
       <c r="M25" t="n">
+        <v>108.825</v>
+      </c>
+      <c r="N25" t="n">
+        <v>225918.75</v>
+      </c>
+      <c r="O25" t="n">
         <v>4461.3</v>
       </c>
-      <c r="N25" t="n">
+      <c r="P25" t="n">
         <v>1</v>
       </c>
-      <c r="O25" t="n">
+      <c r="Q25" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1762,12 +1916,18 @@
         <v>615.7</v>
       </c>
       <c r="M26" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="N26" t="n">
+        <v>223642</v>
+      </c>
+      <c r="O26" t="n">
         <v>4457.6</v>
       </c>
-      <c r="N26" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" t="n">
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1809,12 +1969,18 @@
         <v>615.3</v>
       </c>
       <c r="M27" t="n">
+        <v>136.4</v>
+      </c>
+      <c r="N27" t="n">
+        <v>222562.25</v>
+      </c>
+      <c r="O27" t="n">
         <v>4385.45</v>
       </c>
-      <c r="N27" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" t="n">
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1856,12 +2022,18 @@
         <v>346.8</v>
       </c>
       <c r="M28" t="n">
+        <v>147.4</v>
+      </c>
+      <c r="N28" t="n">
+        <v>215723.25</v>
+      </c>
+      <c r="O28" t="n">
         <v>4126.675</v>
       </c>
-      <c r="N28" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" t="n">
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1903,12 +2075,18 @@
         <v>448.25</v>
       </c>
       <c r="M29" t="n">
+        <v>127.65</v>
+      </c>
+      <c r="N29" t="n">
+        <v>222985.5</v>
+      </c>
+      <c r="O29" t="n">
         <v>4024.95</v>
       </c>
-      <c r="N29" t="n">
+      <c r="P29" t="n">
         <v>4</v>
       </c>
-      <c r="O29" t="n">
+      <c r="Q29" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1950,12 +2128,18 @@
         <v>413.35</v>
       </c>
       <c r="M30" t="n">
+        <v>116.075</v>
+      </c>
+      <c r="N30" t="n">
+        <v>232420.75</v>
+      </c>
+      <c r="O30" t="n">
         <v>3914.525</v>
       </c>
-      <c r="N30" t="n">
+      <c r="P30" t="n">
         <v>4</v>
       </c>
-      <c r="O30" t="n">
+      <c r="Q30" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1997,12 +2181,18 @@
         <v>618.95</v>
       </c>
       <c r="M31" t="n">
+        <v>120.55</v>
+      </c>
+      <c r="N31" t="n">
+        <v>239291</v>
+      </c>
+      <c r="O31" t="n">
         <v>4142</v>
       </c>
-      <c r="N31" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" t="n">
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2044,12 +2234,18 @@
         <v>598.825</v>
       </c>
       <c r="M32" t="n">
+        <v>134.525</v>
+      </c>
+      <c r="N32" t="n">
+        <v>234154.75</v>
+      </c>
+      <c r="O32" t="n">
         <v>4203.700000000001</v>
       </c>
-      <c r="N32" t="n">
-        <v>0</v>
-      </c>
-      <c r="O32" t="n">
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2091,12 +2287,18 @@
         <v>558.45</v>
       </c>
       <c r="M33" t="n">
+        <v>152.775</v>
+      </c>
+      <c r="N33" t="n">
+        <v>232150.5</v>
+      </c>
+      <c r="O33" t="n">
         <v>4215.625</v>
       </c>
-      <c r="N33" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" t="n">
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2138,12 +2340,18 @@
         <v>669.175</v>
       </c>
       <c r="M34" t="n">
+        <v>150.7</v>
+      </c>
+      <c r="N34" t="n">
+        <v>229593.75</v>
+      </c>
+      <c r="O34" t="n">
         <v>4269.1</v>
       </c>
-      <c r="N34" t="n">
-        <v>0</v>
-      </c>
-      <c r="O34" t="n">
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2185,12 +2393,18 @@
         <v>131.2</v>
       </c>
       <c r="M35" t="n">
+        <v>151.725</v>
+      </c>
+      <c r="N35" t="n">
+        <v>224954.25</v>
+      </c>
+      <c r="O35" t="n">
         <v>3785</v>
       </c>
-      <c r="N35" t="n">
-        <v>0</v>
-      </c>
-      <c r="O35" t="n">
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2232,12 +2446,18 @@
         <v>555.45</v>
       </c>
       <c r="M36" t="n">
+        <v>105.725</v>
+      </c>
+      <c r="N36" t="n">
+        <v>232047.75</v>
+      </c>
+      <c r="O36" t="n">
         <v>3993.65</v>
       </c>
-      <c r="N36" t="n">
-        <v>0</v>
-      </c>
-      <c r="O36" t="n">
+      <c r="P36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2279,12 +2499,18 @@
         <v>352.4</v>
       </c>
       <c r="M37" t="n">
+        <v>70.64999999999999</v>
+      </c>
+      <c r="N37" t="n">
+        <v>231800.5</v>
+      </c>
+      <c r="O37" t="n">
         <v>3897.8</v>
       </c>
-      <c r="N37" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" t="n">
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2326,12 +2552,18 @@
         <v>694.6</v>
       </c>
       <c r="M38" t="n">
+        <v>67.19999999999999</v>
+      </c>
+      <c r="N38" t="n">
+        <v>238876</v>
+      </c>
+      <c r="O38" t="n">
         <v>4179.05</v>
       </c>
-      <c r="N38" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" t="n">
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2373,12 +2605,18 @@
         <v>699.325</v>
       </c>
       <c r="M39" t="n">
+        <v>82.44999999999999</v>
+      </c>
+      <c r="N39" t="n">
+        <v>228827.75</v>
+      </c>
+      <c r="O39" t="n">
         <v>4259.425</v>
       </c>
-      <c r="N39" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" t="n">
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2420,12 +2658,18 @@
         <v>305.725</v>
       </c>
       <c r="M40" t="n">
+        <v>83.27499999999999</v>
+      </c>
+      <c r="N40" t="n">
+        <v>219318.75</v>
+      </c>
+      <c r="O40" t="n">
         <v>3966.325</v>
       </c>
-      <c r="N40" t="n">
-        <v>0</v>
-      </c>
-      <c r="O40" t="n">
+      <c r="P40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="n">
         <v>4</v>
       </c>
     </row>
@@ -2467,12 +2711,18 @@
         <v>665.075</v>
       </c>
       <c r="M41" t="n">
+        <v>119.9</v>
+      </c>
+      <c r="N41" t="n">
+        <v>213947</v>
+      </c>
+      <c r="O41" t="n">
         <v>4072.95</v>
       </c>
-      <c r="N41" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" t="n">
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2514,12 +2764,18 @@
         <v>682.85</v>
       </c>
       <c r="M42" t="n">
+        <v>111.9</v>
+      </c>
+      <c r="N42" t="n">
+        <v>209359.5</v>
+      </c>
+      <c r="O42" t="n">
         <v>4086.625</v>
       </c>
-      <c r="N42" t="n">
-        <v>0</v>
-      </c>
-      <c r="O42" t="n">
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2561,12 +2817,18 @@
         <v>640.35</v>
       </c>
       <c r="M43" t="n">
+        <v>93.84999999999999</v>
+      </c>
+      <c r="N43" t="n">
+        <v>207055.25</v>
+      </c>
+      <c r="O43" t="n">
         <v>4595.775000000001</v>
       </c>
-      <c r="N43" t="n">
-        <v>0</v>
-      </c>
-      <c r="O43" t="n">
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2608,12 +2870,18 @@
         <v>773.95</v>
       </c>
       <c r="M44" t="n">
+        <v>92.22499999999999</v>
+      </c>
+      <c r="N44" t="n">
+        <v>207628.5</v>
+      </c>
+      <c r="O44" t="n">
         <v>4814.275000000001</v>
       </c>
-      <c r="N44" t="n">
-        <v>0</v>
-      </c>
-      <c r="O44" t="n">
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2655,12 +2923,18 @@
         <v>841.875</v>
       </c>
       <c r="M45" t="n">
+        <v>81.02500000000001</v>
+      </c>
+      <c r="N45" t="n">
+        <v>210802</v>
+      </c>
+      <c r="O45" t="n">
         <v>5303.750000000001</v>
       </c>
-      <c r="N45" t="n">
-        <v>0</v>
-      </c>
-      <c r="O45" t="n">
+      <c r="P45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2702,12 +2976,18 @@
         <v>734.475</v>
       </c>
       <c r="M46" t="n">
+        <v>116.125</v>
+      </c>
+      <c r="N46" t="n">
+        <v>199988.75</v>
+      </c>
+      <c r="O46" t="n">
         <v>5343.625</v>
       </c>
-      <c r="N46" t="n">
-        <v>0</v>
-      </c>
-      <c r="O46" t="n">
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2749,12 +3029,18 @@
         <v>717.3</v>
       </c>
       <c r="M47" t="n">
+        <v>122.25</v>
+      </c>
+      <c r="N47" t="n">
+        <v>199650.75</v>
+      </c>
+      <c r="O47" t="n">
         <v>5361.6</v>
       </c>
-      <c r="N47" t="n">
-        <v>0</v>
-      </c>
-      <c r="O47" t="n">
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2796,12 +3082,18 @@
         <v>679.45</v>
       </c>
       <c r="M48" t="n">
+        <v>128.6</v>
+      </c>
+      <c r="N48" t="n">
+        <v>197843.5</v>
+      </c>
+      <c r="O48" t="n">
         <v>5735.325</v>
       </c>
-      <c r="N48" t="n">
-        <v>0</v>
-      </c>
-      <c r="O48" t="n">
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2843,12 +3135,18 @@
         <v>617.25</v>
       </c>
       <c r="M49" t="n">
+        <v>123.85</v>
+      </c>
+      <c r="N49" t="n">
+        <v>196727.75</v>
+      </c>
+      <c r="O49" t="n">
         <v>5687.5</v>
       </c>
-      <c r="N49" t="n">
-        <v>0</v>
-      </c>
-      <c r="O49" t="n">
+      <c r="P49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2890,12 +3188,18 @@
         <v>810.025</v>
       </c>
       <c r="M50" t="n">
+        <v>102.025</v>
+      </c>
+      <c r="N50" t="n">
+        <v>200216</v>
+      </c>
+      <c r="O50" t="n">
         <v>5814.675</v>
       </c>
-      <c r="N50" t="n">
-        <v>0</v>
-      </c>
-      <c r="O50" t="n">
+      <c r="P50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q50" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2937,12 +3241,18 @@
         <v>766.2</v>
       </c>
       <c r="M51" t="n">
+        <v>101.05</v>
+      </c>
+      <c r="N51" t="n">
+        <v>199370.25</v>
+      </c>
+      <c r="O51" t="n">
         <v>5940.525000000001</v>
       </c>
-      <c r="N51" t="n">
-        <v>0</v>
-      </c>
-      <c r="O51" t="n">
+      <c r="P51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2984,12 +3294,18 @@
         <v>611.95</v>
       </c>
       <c r="M52" t="n">
+        <v>132</v>
+      </c>
+      <c r="N52" t="n">
+        <v>193086</v>
+      </c>
+      <c r="O52" t="n">
         <v>5778.525</v>
       </c>
-      <c r="N52" t="n">
-        <v>0</v>
-      </c>
-      <c r="O52" t="n">
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3031,12 +3347,18 @@
         <v>657.5</v>
       </c>
       <c r="M53" t="n">
+        <v>141.725</v>
+      </c>
+      <c r="N53" t="n">
+        <v>191337.25</v>
+      </c>
+      <c r="O53" t="n">
         <v>5594.15</v>
       </c>
-      <c r="N53" t="n">
-        <v>0</v>
-      </c>
-      <c r="O53" t="n">
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3076,12 +3398,18 @@
         <v>666.225</v>
       </c>
       <c r="M54" t="n">
+        <v>133.75</v>
+      </c>
+      <c r="N54" t="n">
+        <v>190323.75</v>
+      </c>
+      <c r="O54" t="n">
         <v>5525.900000000001</v>
       </c>
-      <c r="N54" t="n">
-        <v>0</v>
-      </c>
-      <c r="O54" t="n">
+      <c r="P54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q54" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3123,12 +3451,18 @@
         <v>776.75</v>
       </c>
       <c r="M55" t="n">
+        <v>129.275</v>
+      </c>
+      <c r="N55" t="n">
+        <v>192076.75</v>
+      </c>
+      <c r="O55" t="n">
         <v>5585.35</v>
       </c>
-      <c r="N55" t="n">
-        <v>0</v>
-      </c>
-      <c r="O55" t="n">
+      <c r="P55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3170,12 +3504,18 @@
         <v>633.9</v>
       </c>
       <c r="M56" t="n">
+        <v>118.075</v>
+      </c>
+      <c r="N56" t="n">
+        <v>190882.75</v>
+      </c>
+      <c r="O56" t="n">
         <v>5539.8</v>
       </c>
-      <c r="N56" t="n">
-        <v>0</v>
-      </c>
-      <c r="O56" t="n">
+      <c r="P56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q56" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3217,12 +3557,18 @@
         <v>610.575</v>
       </c>
       <c r="M57" t="n">
+        <v>119.95</v>
+      </c>
+      <c r="N57" t="n">
+        <v>191397.5</v>
+      </c>
+      <c r="O57" t="n">
         <v>5533.125</v>
       </c>
-      <c r="N57" t="n">
-        <v>0</v>
-      </c>
-      <c r="O57" t="n">
+      <c r="P57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q57" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3264,12 +3610,18 @@
         <v>742.675</v>
       </c>
       <c r="M58" t="n">
+        <v>150.775</v>
+      </c>
+      <c r="N58" t="n">
+        <v>192559.5</v>
+      </c>
+      <c r="O58" t="n">
         <v>5465.775</v>
       </c>
-      <c r="N58" t="n">
-        <v>0</v>
-      </c>
-      <c r="O58" t="n">
+      <c r="P58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3311,12 +3663,18 @@
         <v>705.7</v>
       </c>
       <c r="M59" t="n">
+        <v>151.675</v>
+      </c>
+      <c r="N59" t="n">
+        <v>199419.5</v>
+      </c>
+      <c r="O59" t="n">
         <v>5405.275</v>
       </c>
-      <c r="N59" t="n">
+      <c r="P59" t="n">
         <v>1</v>
       </c>
-      <c r="O59" t="n">
+      <c r="Q59" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3358,12 +3716,18 @@
         <v>704.625</v>
       </c>
       <c r="M60" t="n">
+        <v>134.55</v>
+      </c>
+      <c r="N60" t="n">
+        <v>207409.75</v>
+      </c>
+      <c r="O60" t="n">
         <v>5497.95</v>
       </c>
-      <c r="N60" t="n">
-        <v>0</v>
-      </c>
-      <c r="O60" t="n">
+      <c r="P60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3405,12 +3769,18 @@
         <v>611.975</v>
       </c>
       <c r="M61" t="n">
+        <v>118.25</v>
+      </c>
+      <c r="N61" t="n">
+        <v>211909.75</v>
+      </c>
+      <c r="O61" t="n">
         <v>5452.425</v>
       </c>
-      <c r="N61" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" t="n">
+      <c r="P61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3452,12 +3822,18 @@
         <v>601.85</v>
       </c>
       <c r="M62" t="n">
+        <v>108.875</v>
+      </c>
+      <c r="N62" t="n">
+        <v>217441.25</v>
+      </c>
+      <c r="O62" t="n">
         <v>5388.05</v>
       </c>
-      <c r="N62" t="n">
+      <c r="P62" t="n">
         <v>2</v>
       </c>
-      <c r="O62" t="n">
+      <c r="Q62" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3499,12 +3875,18 @@
         <v>582.375</v>
       </c>
       <c r="M63" t="n">
+        <v>106.075</v>
+      </c>
+      <c r="N63" t="n">
+        <v>222838</v>
+      </c>
+      <c r="O63" t="n">
         <v>5193.675</v>
       </c>
-      <c r="N63" t="n">
+      <c r="P63" t="n">
         <v>1</v>
       </c>
-      <c r="O63" t="n">
+      <c r="Q63" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3546,12 +3928,18 @@
         <v>718.65</v>
       </c>
       <c r="M64" t="n">
+        <v>103.3</v>
+      </c>
+      <c r="N64" t="n">
+        <v>231075.25</v>
+      </c>
+      <c r="O64" t="n">
         <v>5278.425</v>
       </c>
-      <c r="N64" t="n">
-        <v>0</v>
-      </c>
-      <c r="O64" t="n">
+      <c r="P64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3593,12 +3981,18 @@
         <v>745.875</v>
       </c>
       <c r="M65" t="n">
+        <v>126.825</v>
+      </c>
+      <c r="N65" t="n">
+        <v>232812</v>
+      </c>
+      <c r="O65" t="n">
         <v>5413.725</v>
       </c>
-      <c r="N65" t="n">
-        <v>0</v>
-      </c>
-      <c r="O65" t="n">
+      <c r="P65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q65" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3640,12 +4034,18 @@
         <v>803.9</v>
       </c>
       <c r="M66" t="n">
+        <v>132.8</v>
+      </c>
+      <c r="N66" t="n">
+        <v>237389</v>
+      </c>
+      <c r="O66" t="n">
         <v>5474.95</v>
       </c>
-      <c r="N66" t="n">
-        <v>0</v>
-      </c>
-      <c r="O66" t="n">
+      <c r="P66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3687,12 +4087,18 @@
         <v>656.25</v>
       </c>
       <c r="M67" t="n">
+        <v>100.25</v>
+      </c>
+      <c r="N67" t="n">
+        <v>234887.25</v>
+      </c>
+      <c r="O67" t="n">
         <v>5425.5</v>
       </c>
-      <c r="N67" t="n">
-        <v>0</v>
-      </c>
-      <c r="O67" t="n">
+      <c r="P67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3734,12 +4140,18 @@
         <v>739.025</v>
       </c>
       <c r="M68" t="n">
+        <v>157.05</v>
+      </c>
+      <c r="N68" t="n">
+        <v>229690.75</v>
+      </c>
+      <c r="O68" t="n">
         <v>5459.900000000001</v>
       </c>
-      <c r="N68" t="n">
-        <v>0</v>
-      </c>
-      <c r="O68" t="n">
+      <c r="P68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3781,12 +4193,18 @@
         <v>749.925</v>
       </c>
       <c r="M69" t="n">
+        <v>188.25</v>
+      </c>
+      <c r="N69" t="n">
+        <v>220164.75</v>
+      </c>
+      <c r="O69" t="n">
         <v>5597.85</v>
       </c>
-      <c r="N69" t="n">
-        <v>0</v>
-      </c>
-      <c r="O69" t="n">
+      <c r="P69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3828,12 +4246,18 @@
         <v>855.35</v>
       </c>
       <c r="M70" t="n">
+        <v>190.475</v>
+      </c>
+      <c r="N70" t="n">
+        <v>218533.5</v>
+      </c>
+      <c r="O70" t="n">
         <v>5851.349999999999</v>
       </c>
-      <c r="N70" t="n">
-        <v>0</v>
-      </c>
-      <c r="O70" t="n">
+      <c r="P70" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q70" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3875,12 +4299,18 @@
         <v>872.2</v>
       </c>
       <c r="M71" t="n">
+        <v>201.375</v>
+      </c>
+      <c r="N71" t="n">
+        <v>226476.5</v>
+      </c>
+      <c r="O71" t="n">
         <v>6141.174999999999</v>
       </c>
-      <c r="N71" t="n">
-        <v>0</v>
-      </c>
-      <c r="O71" t="n">
+      <c r="P71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q71" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3922,12 +4352,18 @@
         <v>674.525</v>
       </c>
       <c r="M72" t="n">
+        <v>177.575</v>
+      </c>
+      <c r="N72" t="n">
+        <v>223833.5</v>
+      </c>
+      <c r="O72" t="n">
         <v>6097.05</v>
       </c>
-      <c r="N72" t="n">
-        <v>0</v>
-      </c>
-      <c r="O72" t="n">
+      <c r="P72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3969,12 +4405,18 @@
         <v>624.375</v>
       </c>
       <c r="M73" t="n">
+        <v>167.2</v>
+      </c>
+      <c r="N73" t="n">
+        <v>225631</v>
+      </c>
+      <c r="O73" t="n">
         <v>5975.55</v>
       </c>
-      <c r="N73" t="n">
+      <c r="P73" t="n">
         <v>2</v>
       </c>
-      <c r="O73" t="n">
+      <c r="Q73" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4016,12 +4458,18 @@
         <v>596.95</v>
       </c>
       <c r="M74" t="n">
+        <v>130.975</v>
+      </c>
+      <c r="N74" t="n">
+        <v>226517.75</v>
+      </c>
+      <c r="O74" t="n">
         <v>5768.6</v>
       </c>
-      <c r="N74" t="n">
-        <v>0</v>
-      </c>
-      <c r="O74" t="n">
+      <c r="P74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4063,12 +4511,18 @@
         <v>797.775</v>
       </c>
       <c r="M75" t="n">
+        <v>129.675</v>
+      </c>
+      <c r="N75" t="n">
+        <v>224364</v>
+      </c>
+      <c r="O75" t="n">
         <v>5910.125</v>
       </c>
-      <c r="N75" t="n">
-        <v>0</v>
-      </c>
-      <c r="O75" t="n">
+      <c r="P75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4110,12 +4564,18 @@
         <v>820.575</v>
       </c>
       <c r="M76" t="n">
+        <v>117.825</v>
+      </c>
+      <c r="N76" t="n">
+        <v>225983.5</v>
+      </c>
+      <c r="O76" t="n">
         <v>5991.675</v>
       </c>
-      <c r="N76" t="n">
-        <v>0</v>
-      </c>
-      <c r="O76" t="n">
+      <c r="P76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4157,12 +4617,18 @@
         <v>863.15</v>
       </c>
       <c r="M77" t="n">
+        <v>94.27499999999999</v>
+      </c>
+      <c r="N77" t="n">
+        <v>226335.25</v>
+      </c>
+      <c r="O77" t="n">
         <v>6104.9</v>
       </c>
-      <c r="N77" t="n">
-        <v>0</v>
-      </c>
-      <c r="O77" t="n">
+      <c r="P77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4204,12 +4670,18 @@
         <v>718.375</v>
       </c>
       <c r="M78" t="n">
+        <v>59.075</v>
+      </c>
+      <c r="N78" t="n">
+        <v>242668</v>
+      </c>
+      <c r="O78" t="n">
         <v>5967.925</v>
       </c>
-      <c r="N78" t="n">
+      <c r="P78" t="n">
         <v>2</v>
       </c>
-      <c r="O78" t="n">
+      <c r="Q78" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4251,12 +4723,18 @@
         <v>688.975</v>
       </c>
       <c r="M79" t="n">
+        <v>64.8</v>
+      </c>
+      <c r="N79" t="n">
+        <v>252542.5</v>
+      </c>
+      <c r="O79" t="n">
         <v>5784.700000000001</v>
       </c>
-      <c r="N79" t="n">
+      <c r="P79" t="n">
         <v>2</v>
       </c>
-      <c r="O79" t="n">
+      <c r="Q79" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4298,12 +4776,18 @@
         <v>655.2</v>
       </c>
       <c r="M80" t="n">
+        <v>54</v>
+      </c>
+      <c r="N80" t="n">
+        <v>254270.75</v>
+      </c>
+      <c r="O80" t="n">
         <v>5765.375</v>
       </c>
-      <c r="N80" t="n">
-        <v>0</v>
-      </c>
-      <c r="O80" t="n">
+      <c r="P80" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q80" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4345,12 +4829,18 @@
         <v>699.575</v>
       </c>
       <c r="M81" t="n">
+        <v>54</v>
+      </c>
+      <c r="N81" t="n">
+        <v>267029</v>
+      </c>
+      <c r="O81" t="n">
         <v>5840.575</v>
       </c>
-      <c r="N81" t="n">
+      <c r="P81" t="n">
         <v>3</v>
       </c>
-      <c r="O81" t="n">
+      <c r="Q81" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4392,12 +4882,18 @@
         <v>900.625</v>
       </c>
       <c r="M82" t="n">
+        <v>63.47499999999999</v>
+      </c>
+      <c r="N82" t="n">
+        <v>265424.75</v>
+      </c>
+      <c r="O82" t="n">
         <v>6144.25</v>
       </c>
-      <c r="N82" t="n">
-        <v>0</v>
-      </c>
-      <c r="O82" t="n">
+      <c r="P82" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q82" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4439,12 +4935,18 @@
         <v>631.65</v>
       </c>
       <c r="M83" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="N83" t="n">
+        <v>258239.25</v>
+      </c>
+      <c r="O83" t="n">
         <v>5978.125</v>
       </c>
-      <c r="N83" t="n">
-        <v>0</v>
-      </c>
-      <c r="O83" t="n">
+      <c r="P83" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q83" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4486,12 +4988,18 @@
         <v>786</v>
       </c>
       <c r="M84" t="n">
+        <v>55.72499999999999</v>
+      </c>
+      <c r="N84" t="n">
+        <v>262936.75</v>
+      </c>
+      <c r="O84" t="n">
         <v>5943.549999999999</v>
       </c>
-      <c r="N84" t="n">
-        <v>0</v>
-      </c>
-      <c r="O84" t="n">
+      <c r="P84" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4533,12 +5041,18 @@
         <v>689.975</v>
       </c>
       <c r="M85" t="n">
+        <v>43.375</v>
+      </c>
+      <c r="N85" t="n">
+        <v>276732</v>
+      </c>
+      <c r="O85" t="n">
         <v>5770.375</v>
       </c>
-      <c r="N85" t="n">
+      <c r="P85" t="n">
         <v>1</v>
       </c>
-      <c r="O85" t="n">
+      <c r="Q85" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4580,12 +5094,18 @@
         <v>674.025</v>
       </c>
       <c r="M86" t="n">
+        <v>44.875</v>
+      </c>
+      <c r="N86" t="n">
+        <v>271848.5</v>
+      </c>
+      <c r="O86" t="n">
         <v>5726.025</v>
       </c>
-      <c r="N86" t="n">
-        <v>0</v>
-      </c>
-      <c r="O86" t="n">
+      <c r="P86" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4627,12 +5147,18 @@
         <v>921.25</v>
       </c>
       <c r="M87" t="n">
+        <v>38.25</v>
+      </c>
+      <c r="N87" t="n">
+        <v>260605.75</v>
+      </c>
+      <c r="O87" t="n">
         <v>5958.299999999999</v>
       </c>
-      <c r="N87" t="n">
-        <v>0</v>
-      </c>
-      <c r="O87" t="n">
+      <c r="P87" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4674,12 +5200,18 @@
         <v>890.475</v>
       </c>
       <c r="M88" t="n">
+        <v>37.15</v>
+      </c>
+      <c r="N88" t="n">
+        <v>247545.75</v>
+      </c>
+      <c r="O88" t="n">
         <v>6193.575</v>
       </c>
-      <c r="N88" t="n">
-        <v>0</v>
-      </c>
-      <c r="O88" t="n">
+      <c r="P88" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q88" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4721,12 +5253,18 @@
         <v>945.475</v>
       </c>
       <c r="M89" t="n">
+        <v>38.8</v>
+      </c>
+      <c r="N89" t="n">
+        <v>243969.75</v>
+      </c>
+      <c r="O89" t="n">
         <v>6439.475</v>
       </c>
-      <c r="N89" t="n">
-        <v>0</v>
-      </c>
-      <c r="O89" t="n">
+      <c r="P89" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q89" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4768,12 +5306,18 @@
         <v>778.075</v>
       </c>
       <c r="M90" t="n">
+        <v>40.1</v>
+      </c>
+      <c r="N90" t="n">
+        <v>235278</v>
+      </c>
+      <c r="O90" t="n">
         <v>6316.925</v>
       </c>
-      <c r="N90" t="n">
-        <v>0</v>
-      </c>
-      <c r="O90" t="n">
+      <c r="P90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4815,12 +5359,18 @@
         <v>743.975</v>
       </c>
       <c r="M91" t="n">
+        <v>18.85</v>
+      </c>
+      <c r="N91" t="n">
+        <v>233199.75</v>
+      </c>
+      <c r="O91" t="n">
         <v>6429.25</v>
       </c>
-      <c r="N91" t="n">
-        <v>0</v>
-      </c>
-      <c r="O91" t="n">
+      <c r="P91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4862,12 +5412,18 @@
         <v>829.3</v>
       </c>
       <c r="M92" t="n">
+        <v>18.85</v>
+      </c>
+      <c r="N92" t="n">
+        <v>242974</v>
+      </c>
+      <c r="O92" t="n">
         <v>6472.549999999999</v>
       </c>
-      <c r="N92" t="n">
+      <c r="P92" t="n">
         <v>1</v>
       </c>
-      <c r="O92" t="n">
+      <c r="Q92" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4909,12 +5465,18 @@
         <v>892.65</v>
       </c>
       <c r="M93" t="n">
+        <v>42.675</v>
+      </c>
+      <c r="N93" t="n">
+        <v>236116.75</v>
+      </c>
+      <c r="O93" t="n">
         <v>6675.225</v>
       </c>
-      <c r="N93" t="n">
-        <v>0</v>
-      </c>
-      <c r="O93" t="n">
+      <c r="P93" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="n">
         <v>7</v>
       </c>
     </row>
@@ -4956,12 +5518,18 @@
         <v>895.575</v>
       </c>
       <c r="M94" t="n">
+        <v>59.75</v>
+      </c>
+      <c r="N94" t="n">
+        <v>223603.75</v>
+      </c>
+      <c r="O94" t="n">
         <v>6896.775000000001</v>
       </c>
-      <c r="N94" t="n">
-        <v>0</v>
-      </c>
-      <c r="O94" t="n">
+      <c r="P94" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5003,12 +5571,18 @@
         <v>827.1</v>
       </c>
       <c r="M95" t="n">
+        <v>88.34999999999999</v>
+      </c>
+      <c r="N95" t="n">
+        <v>217403.5</v>
+      </c>
+      <c r="O95" t="n">
         <v>6802.625</v>
       </c>
-      <c r="N95" t="n">
-        <v>0</v>
-      </c>
-      <c r="O95" t="n">
+      <c r="P95" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5050,12 +5624,18 @@
         <v>941.075</v>
       </c>
       <c r="M96" t="n">
+        <v>130.45</v>
+      </c>
+      <c r="N96" t="n">
+        <v>215560.25</v>
+      </c>
+      <c r="O96" t="n">
         <v>6853.225</v>
       </c>
-      <c r="N96" t="n">
-        <v>0</v>
-      </c>
-      <c r="O96" t="n">
+      <c r="P96" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5097,12 +5677,18 @@
         <v>880.025</v>
       </c>
       <c r="M97" t="n">
+        <v>138.525</v>
+      </c>
+      <c r="N97" t="n">
+        <v>215349.25</v>
+      </c>
+      <c r="O97" t="n">
         <v>6787.775</v>
       </c>
-      <c r="N97" t="n">
-        <v>0</v>
-      </c>
-      <c r="O97" t="n">
+      <c r="P97" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5144,12 +5730,18 @@
         <v>835.775</v>
       </c>
       <c r="M98" t="n">
+        <v>141.625</v>
+      </c>
+      <c r="N98" t="n">
+        <v>203391.25</v>
+      </c>
+      <c r="O98" t="n">
         <v>6845.475</v>
       </c>
-      <c r="N98" t="n">
-        <v>0</v>
-      </c>
-      <c r="O98" t="n">
+      <c r="P98" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5191,12 +5783,18 @@
         <v>789.125</v>
       </c>
       <c r="M99" t="n">
+        <v>161.875</v>
+      </c>
+      <c r="N99" t="n">
+        <v>202571.5</v>
+      </c>
+      <c r="O99" t="n">
         <v>6890.625</v>
       </c>
-      <c r="N99" t="n">
-        <v>0</v>
-      </c>
-      <c r="O99" t="n">
+      <c r="P99" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q99" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5238,12 +5836,18 @@
         <v>819.825</v>
       </c>
       <c r="M100" t="n">
+        <v>178.425</v>
+      </c>
+      <c r="N100" t="n">
+        <v>198492.5</v>
+      </c>
+      <c r="O100" t="n">
         <v>6881.150000000001</v>
       </c>
-      <c r="N100" t="n">
-        <v>0</v>
-      </c>
-      <c r="O100" t="n">
+      <c r="P100" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5285,12 +5889,18 @@
         <v>332.425</v>
       </c>
       <c r="M101" t="n">
+        <v>201.825</v>
+      </c>
+      <c r="N101" t="n">
+        <v>173718</v>
+      </c>
+      <c r="O101" t="n">
         <v>6320.925</v>
       </c>
-      <c r="N101" t="n">
-        <v>0</v>
-      </c>
-      <c r="O101" t="n">
+      <c r="P101" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q101" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5332,12 +5942,18 @@
         <v>600.025</v>
       </c>
       <c r="M102" t="n">
+        <v>198.225</v>
+      </c>
+      <c r="N102" t="n">
+        <v>170984</v>
+      </c>
+      <c r="O102" t="n">
         <v>6025.375</v>
       </c>
-      <c r="N102" t="n">
-        <v>0</v>
-      </c>
-      <c r="O102" t="n">
+      <c r="P102" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q102" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5379,12 +5995,18 @@
         <v>630.45</v>
       </c>
       <c r="M103" t="n">
+        <v>178.7</v>
+      </c>
+      <c r="N103" t="n">
+        <v>171337.75</v>
+      </c>
+      <c r="O103" t="n">
         <v>5828.724999999999</v>
       </c>
-      <c r="N103" t="n">
-        <v>0</v>
-      </c>
-      <c r="O103" t="n">
+      <c r="P103" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q103" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5426,12 +6048,18 @@
         <v>751.95</v>
       </c>
       <c r="M104" t="n">
+        <v>174.3</v>
+      </c>
+      <c r="N104" t="n">
+        <v>172034</v>
+      </c>
+      <c r="O104" t="n">
         <v>5639.6</v>
       </c>
-      <c r="N104" t="n">
-        <v>0</v>
-      </c>
-      <c r="O104" t="n">
+      <c r="P104" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q104" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5473,12 +6101,18 @@
         <v>204.6</v>
       </c>
       <c r="M105" t="n">
+        <v>154.875</v>
+      </c>
+      <c r="N105" t="n">
+        <v>175835.5</v>
+      </c>
+      <c r="O105" t="n">
         <v>4964.175</v>
       </c>
-      <c r="N105" t="n">
-        <v>0</v>
-      </c>
-      <c r="O105" t="n">
+      <c r="P105" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5520,12 +6154,18 @@
         <v>666.85</v>
       </c>
       <c r="M106" t="n">
+        <v>132.35</v>
+      </c>
+      <c r="N106" t="n">
+        <v>178857</v>
+      </c>
+      <c r="O106" t="n">
         <v>4795.25</v>
       </c>
-      <c r="N106" t="n">
-        <v>0</v>
-      </c>
-      <c r="O106" t="n">
+      <c r="P106" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q106" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5567,12 +6207,18 @@
         <v>579.25</v>
       </c>
       <c r="M107" t="n">
+        <v>128.45</v>
+      </c>
+      <c r="N107" t="n">
+        <v>175505</v>
+      </c>
+      <c r="O107" t="n">
         <v>4585.375</v>
       </c>
-      <c r="N107" t="n">
-        <v>0</v>
-      </c>
-      <c r="O107" t="n">
+      <c r="P107" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q107" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5614,12 +6260,18 @@
         <v>649.925</v>
       </c>
       <c r="M108" t="n">
+        <v>94.89999999999999</v>
+      </c>
+      <c r="N108" t="n">
+        <v>185839.75</v>
+      </c>
+      <c r="O108" t="n">
         <v>4415.475</v>
       </c>
-      <c r="N108" t="n">
-        <v>0</v>
-      </c>
-      <c r="O108" t="n">
+      <c r="P108" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q108" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5661,12 +6313,18 @@
         <v>822.775</v>
       </c>
       <c r="M109" t="n">
+        <v>83.125</v>
+      </c>
+      <c r="N109" t="n">
+        <v>189373.75</v>
+      </c>
+      <c r="O109" t="n">
         <v>4905.825</v>
       </c>
-      <c r="N109" t="n">
-        <v>0</v>
-      </c>
-      <c r="O109" t="n">
+      <c r="P109" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q109" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5708,12 +6366,18 @@
         <v>781.025</v>
       </c>
       <c r="M110" t="n">
+        <v>66.55</v>
+      </c>
+      <c r="N110" t="n">
+        <v>205844.25</v>
+      </c>
+      <c r="O110" t="n">
         <v>5086.825</v>
       </c>
-      <c r="N110" t="n">
-        <v>0</v>
-      </c>
-      <c r="O110" t="n">
+      <c r="P110" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q110" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5755,12 +6419,18 @@
         <v>811.9</v>
       </c>
       <c r="M111" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="N111" t="n">
+        <v>219091.75</v>
+      </c>
+      <c r="O111" t="n">
         <v>5268.275</v>
       </c>
-      <c r="N111" t="n">
-        <v>0</v>
-      </c>
-      <c r="O111" t="n">
+      <c r="P111" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5802,12 +6472,18 @@
         <v>607.025</v>
       </c>
       <c r="M112" t="n">
+        <v>45.975</v>
+      </c>
+      <c r="N112" t="n">
+        <v>228351.5</v>
+      </c>
+      <c r="O112" t="n">
         <v>5123.35</v>
       </c>
-      <c r="N112" t="n">
-        <v>0</v>
-      </c>
-      <c r="O112" t="n">
+      <c r="P112" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q112" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5849,12 +6525,18 @@
         <v>634.9</v>
       </c>
       <c r="M113" t="n">
+        <v>49.175</v>
+      </c>
+      <c r="N113" t="n">
+        <v>233790.75</v>
+      </c>
+      <c r="O113" t="n">
         <v>5553.65</v>
       </c>
-      <c r="N113" t="n">
-        <v>0</v>
-      </c>
-      <c r="O113" t="n">
+      <c r="P113" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q113" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5896,12 +6578,18 @@
         <v>682.875</v>
       </c>
       <c r="M114" t="n">
+        <v>76.52499999999999</v>
+      </c>
+      <c r="N114" t="n">
+        <v>235176</v>
+      </c>
+      <c r="O114" t="n">
         <v>5569.675</v>
       </c>
-      <c r="N114" t="n">
+      <c r="P114" t="n">
         <v>1</v>
       </c>
-      <c r="O114" t="n">
+      <c r="Q114" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5943,12 +6631,18 @@
         <v>792.65</v>
       </c>
       <c r="M115" t="n">
+        <v>84.12499999999999</v>
+      </c>
+      <c r="N115" t="n">
+        <v>244599</v>
+      </c>
+      <c r="O115" t="n">
         <v>5783.075</v>
       </c>
-      <c r="N115" t="n">
-        <v>0</v>
-      </c>
-      <c r="O115" t="n">
+      <c r="P115" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q115" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5990,12 +6684,18 @@
         <v>782.875</v>
       </c>
       <c r="M116" t="n">
+        <v>123.8</v>
+      </c>
+      <c r="N116" t="n">
+        <v>249275.75</v>
+      </c>
+      <c r="O116" t="n">
         <v>5916.025</v>
       </c>
-      <c r="N116" t="n">
-        <v>0</v>
-      </c>
-      <c r="O116" t="n">
+      <c r="P116" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q116" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6037,12 +6737,18 @@
         <v>812.925</v>
       </c>
       <c r="M117" t="n">
+        <v>141.575</v>
+      </c>
+      <c r="N117" t="n">
+        <v>246998.25</v>
+      </c>
+      <c r="O117" t="n">
         <v>5906.175</v>
       </c>
-      <c r="N117" t="n">
-        <v>0</v>
-      </c>
-      <c r="O117" t="n">
+      <c r="P117" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q117" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6084,12 +6790,18 @@
         <v>696</v>
       </c>
       <c r="M118" t="n">
+        <v>171.625</v>
+      </c>
+      <c r="N118" t="n">
+        <v>242980.25</v>
+      </c>
+      <c r="O118" t="n">
         <v>5821.15</v>
       </c>
-      <c r="N118" t="n">
-        <v>0</v>
-      </c>
-      <c r="O118" t="n">
+      <c r="P118" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q118" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6131,12 +6843,18 @@
         <v>691.75</v>
       </c>
       <c r="M119" t="n">
+        <v>193.575</v>
+      </c>
+      <c r="N119" t="n">
+        <v>229848.5</v>
+      </c>
+      <c r="O119" t="n">
         <v>5701</v>
       </c>
-      <c r="N119" t="n">
-        <v>0</v>
-      </c>
-      <c r="O119" t="n">
+      <c r="P119" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q119" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6178,12 +6896,18 @@
         <v>697.05</v>
       </c>
       <c r="M120" t="n">
+        <v>263.575</v>
+      </c>
+      <c r="N120" t="n">
+        <v>226183</v>
+      </c>
+      <c r="O120" t="n">
         <v>5791.025000000001</v>
       </c>
-      <c r="N120" t="n">
-        <v>0</v>
-      </c>
-      <c r="O120" t="n">
+      <c r="P120" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q120" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6225,12 +6949,18 @@
         <v>560.725</v>
       </c>
       <c r="M121" t="n">
+        <v>235.725</v>
+      </c>
+      <c r="N121" t="n">
+        <v>228991.25</v>
+      </c>
+      <c r="O121" t="n">
         <v>5716.849999999999</v>
       </c>
-      <c r="N121" t="n">
-        <v>0</v>
-      </c>
-      <c r="O121" t="n">
+      <c r="P121" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q121" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6272,12 +7002,18 @@
         <v>768.575</v>
       </c>
       <c r="M122" t="n">
+        <v>201.775</v>
+      </c>
+      <c r="N122" t="n">
+        <v>232188</v>
+      </c>
+      <c r="O122" t="n">
         <v>5802.55</v>
       </c>
-      <c r="N122" t="n">
-        <v>0</v>
-      </c>
-      <c r="O122" t="n">
+      <c r="P122" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q122" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6319,12 +7055,18 @@
         <v>538.925</v>
       </c>
       <c r="M123" t="n">
+        <v>195.525</v>
+      </c>
+      <c r="N123" t="n">
+        <v>233028.5</v>
+      </c>
+      <c r="O123" t="n">
         <v>5548.825</v>
       </c>
-      <c r="N123" t="n">
-        <v>0</v>
-      </c>
-      <c r="O123" t="n">
+      <c r="P123" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q123" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6366,12 +7108,18 @@
         <v>578.825</v>
       </c>
       <c r="M124" t="n">
+        <v>181.5</v>
+      </c>
+      <c r="N124" t="n">
+        <v>225277</v>
+      </c>
+      <c r="O124" t="n">
         <v>5344.775000000001</v>
       </c>
-      <c r="N124" t="n">
-        <v>0</v>
-      </c>
-      <c r="O124" t="n">
+      <c r="P124" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q124" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6413,12 +7161,18 @@
         <v>744.8000000000001</v>
       </c>
       <c r="M125" t="n">
+        <v>171.425</v>
+      </c>
+      <c r="N125" t="n">
+        <v>224863</v>
+      </c>
+      <c r="O125" t="n">
         <v>5276.65</v>
       </c>
-      <c r="N125" t="n">
-        <v>0</v>
-      </c>
-      <c r="O125" t="n">
+      <c r="P125" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q125" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6460,12 +7214,18 @@
         <v>592.5500000000001</v>
       </c>
       <c r="M126" t="n">
+        <v>152.9</v>
+      </c>
+      <c r="N126" t="n">
+        <v>222317.5</v>
+      </c>
+      <c r="O126" t="n">
         <v>5173.2</v>
       </c>
-      <c r="N126" t="n">
-        <v>0</v>
-      </c>
-      <c r="O126" t="n">
+      <c r="P126" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q126" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6507,12 +7267,18 @@
         <v>689.775</v>
       </c>
       <c r="M127" t="n">
+        <v>133.7</v>
+      </c>
+      <c r="N127" t="n">
+        <v>233778.5</v>
+      </c>
+      <c r="O127" t="n">
         <v>5171.225</v>
       </c>
-      <c r="N127" t="n">
+      <c r="P127" t="n">
         <v>1</v>
       </c>
-      <c r="O127" t="n">
+      <c r="Q127" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6554,12 +7320,18 @@
         <v>490.05</v>
       </c>
       <c r="M128" t="n">
+        <v>75.77500000000001</v>
+      </c>
+      <c r="N128" t="n">
+        <v>248792.75</v>
+      </c>
+      <c r="O128" t="n">
         <v>4964.225</v>
       </c>
-      <c r="N128" t="n">
+      <c r="P128" t="n">
         <v>3</v>
       </c>
-      <c r="O128" t="n">
+      <c r="Q128" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6601,12 +7373,18 @@
         <v>466.6</v>
       </c>
       <c r="M129" t="n">
+        <v>33.375</v>
+      </c>
+      <c r="N129" t="n">
+        <v>257347</v>
+      </c>
+      <c r="O129" t="n">
         <v>4870.1</v>
       </c>
-      <c r="N129" t="n">
+      <c r="P129" t="n">
         <v>3</v>
       </c>
-      <c r="O129" t="n">
+      <c r="Q129" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6648,12 +7426,18 @@
         <v>612.775</v>
       </c>
       <c r="M130" t="n">
+        <v>32.275</v>
+      </c>
+      <c r="N130" t="n">
+        <v>258656.75</v>
+      </c>
+      <c r="O130" t="n">
         <v>4714.299999999999</v>
       </c>
-      <c r="N130" t="n">
-        <v>0</v>
-      </c>
-      <c r="O130" t="n">
+      <c r="P130" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q130" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6695,12 +7479,18 @@
         <v>788.9</v>
       </c>
       <c r="M131" t="n">
+        <v>59.6</v>
+      </c>
+      <c r="N131" t="n">
+        <v>253534</v>
+      </c>
+      <c r="O131" t="n">
         <v>4964.275000000001</v>
       </c>
-      <c r="N131" t="n">
-        <v>0</v>
-      </c>
-      <c r="O131" t="n">
+      <c r="P131" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6742,12 +7532,18 @@
         <v>663.775</v>
       </c>
       <c r="M132" t="n">
+        <v>105.175</v>
+      </c>
+      <c r="N132" t="n">
+        <v>249354.25</v>
+      </c>
+      <c r="O132" t="n">
         <v>5049.224999999999</v>
       </c>
-      <c r="N132" t="n">
-        <v>0</v>
-      </c>
-      <c r="O132" t="n">
+      <c r="P132" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q132" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6789,12 +7585,18 @@
         <v>726.175</v>
       </c>
       <c r="M133" t="n">
+        <v>113.975</v>
+      </c>
+      <c r="N133" t="n">
+        <v>246527.75</v>
+      </c>
+      <c r="O133" t="n">
         <v>5030.599999999999</v>
       </c>
-      <c r="N133" t="n">
-        <v>0</v>
-      </c>
-      <c r="O133" t="n">
+      <c r="P133" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q133" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6836,12 +7638,18 @@
         <v>855.875</v>
       </c>
       <c r="M134" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="N134" t="n">
+        <v>244238.25</v>
+      </c>
+      <c r="O134" t="n">
         <v>5293.925</v>
       </c>
-      <c r="N134" t="n">
-        <v>0</v>
-      </c>
-      <c r="O134" t="n">
+      <c r="P134" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q134" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6883,12 +7691,18 @@
         <v>642.8</v>
       </c>
       <c r="M135" t="n">
+        <v>124.55</v>
+      </c>
+      <c r="N135" t="n">
+        <v>244811</v>
+      </c>
+      <c r="O135" t="n">
         <v>5246.95</v>
       </c>
-      <c r="N135" t="n">
-        <v>0</v>
-      </c>
-      <c r="O135" t="n">
+      <c r="P135" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q135" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6930,12 +7744,18 @@
         <v>722.375</v>
       </c>
       <c r="M136" t="n">
+        <v>152.35</v>
+      </c>
+      <c r="N136" t="n">
+        <v>234230.25</v>
+      </c>
+      <c r="O136" t="n">
         <v>5479.275</v>
       </c>
-      <c r="N136" t="n">
-        <v>0</v>
-      </c>
-      <c r="O136" t="n">
+      <c r="P136" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q136" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6977,12 +7797,18 @@
         <v>656.95</v>
       </c>
       <c r="M137" t="n">
+        <v>172.775</v>
+      </c>
+      <c r="N137" t="n">
+        <v>215063</v>
+      </c>
+      <c r="O137" t="n">
         <v>5669.625</v>
       </c>
-      <c r="N137" t="n">
-        <v>0</v>
-      </c>
-      <c r="O137" t="n">
+      <c r="P137" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q137" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7024,12 +7850,18 @@
         <v>692.225</v>
       </c>
       <c r="M138" t="n">
+        <v>192.225</v>
+      </c>
+      <c r="N138" t="n">
+        <v>219081.5</v>
+      </c>
+      <c r="O138" t="n">
         <v>5749.075000000001</v>
       </c>
-      <c r="N138" t="n">
+      <c r="P138" t="n">
         <v>1</v>
       </c>
-      <c r="O138" t="n">
+      <c r="Q138" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7071,12 +7903,18 @@
         <v>737.675</v>
       </c>
       <c r="M139" t="n">
+        <v>200.5</v>
+      </c>
+      <c r="N139" t="n">
+        <v>216110</v>
+      </c>
+      <c r="O139" t="n">
         <v>5697.849999999999</v>
       </c>
-      <c r="N139" t="n">
-        <v>0</v>
-      </c>
-      <c r="O139" t="n">
+      <c r="P139" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7118,12 +7956,18 @@
         <v>689.925</v>
       </c>
       <c r="M140" t="n">
+        <v>192.975</v>
+      </c>
+      <c r="N140" t="n">
+        <v>219248.5</v>
+      </c>
+      <c r="O140" t="n">
         <v>5724</v>
       </c>
-      <c r="N140" t="n">
-        <v>0</v>
-      </c>
-      <c r="O140" t="n">
+      <c r="P140" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q140" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7165,12 +8009,18 @@
         <v>812.775</v>
       </c>
       <c r="M141" t="n">
+        <v>173.7</v>
+      </c>
+      <c r="N141" t="n">
+        <v>223721.5</v>
+      </c>
+      <c r="O141" t="n">
         <v>5810.6</v>
       </c>
-      <c r="N141" t="n">
-        <v>0</v>
-      </c>
-      <c r="O141" t="n">
+      <c r="P141" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q141" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7212,12 +8062,18 @@
         <v>720.475</v>
       </c>
       <c r="M142" t="n">
+        <v>270.925</v>
+      </c>
+      <c r="N142" t="n">
+        <v>226525.25</v>
+      </c>
+      <c r="O142" t="n">
         <v>5675.2</v>
       </c>
-      <c r="N142" t="n">
-        <v>0</v>
-      </c>
-      <c r="O142" t="n">
+      <c r="P142" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q142" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7259,12 +8115,18 @@
         <v>734.4</v>
       </c>
       <c r="M143" t="n">
+        <v>296.275</v>
+      </c>
+      <c r="N143" t="n">
+        <v>226109</v>
+      </c>
+      <c r="O143" t="n">
         <v>5766.799999999999</v>
       </c>
-      <c r="N143" t="n">
-        <v>0</v>
-      </c>
-      <c r="O143" t="n">
+      <c r="P143" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q143" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7306,12 +8168,18 @@
         <v>606.575</v>
       </c>
       <c r="M144" t="n">
+        <v>262.2</v>
+      </c>
+      <c r="N144" t="n">
+        <v>219515.25</v>
+      </c>
+      <c r="O144" t="n">
         <v>5651</v>
       </c>
-      <c r="N144" t="n">
-        <v>0</v>
-      </c>
-      <c r="O144" t="n">
+      <c r="P144" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q144" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7353,12 +8221,18 @@
         <v>718.025</v>
       </c>
       <c r="M145" t="n">
+        <v>249.8</v>
+      </c>
+      <c r="N145" t="n">
+        <v>214749</v>
+      </c>
+      <c r="O145" t="n">
         <v>5712.075</v>
       </c>
-      <c r="N145" t="n">
-        <v>0</v>
-      </c>
-      <c r="O145" t="n">
+      <c r="P145" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q145" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7400,12 +8274,18 @@
         <v>729.425</v>
       </c>
       <c r="M146" t="n">
+        <v>266.275</v>
+      </c>
+      <c r="N146" t="n">
+        <v>208770.5</v>
+      </c>
+      <c r="O146" t="n">
         <v>5749.275</v>
       </c>
-      <c r="N146" t="n">
-        <v>0</v>
-      </c>
-      <c r="O146" t="n">
+      <c r="P146" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7447,12 +8327,18 @@
         <v>716.35</v>
       </c>
       <c r="M147" t="n">
+        <v>252.05</v>
+      </c>
+      <c r="N147" t="n">
+        <v>207318.5</v>
+      </c>
+      <c r="O147" t="n">
         <v>5727.950000000001</v>
       </c>
-      <c r="N147" t="n">
-        <v>0</v>
-      </c>
-      <c r="O147" t="n">
+      <c r="P147" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q147" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7494,12 +8380,18 @@
         <v>636.625</v>
       </c>
       <c r="M148" t="n">
+        <v>214.35</v>
+      </c>
+      <c r="N148" t="n">
+        <v>205163.5</v>
+      </c>
+      <c r="O148" t="n">
         <v>5674.65</v>
       </c>
-      <c r="N148" t="n">
-        <v>0</v>
-      </c>
-      <c r="O148" t="n">
+      <c r="P148" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q148" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7541,12 +8433,18 @@
         <v>671.15</v>
       </c>
       <c r="M149" t="n">
+        <v>238.4</v>
+      </c>
+      <c r="N149" t="n">
+        <v>195518.5</v>
+      </c>
+      <c r="O149" t="n">
         <v>5533.025000000001</v>
       </c>
-      <c r="N149" t="n">
-        <v>0</v>
-      </c>
-      <c r="O149" t="n">
+      <c r="P149" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q149" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7588,12 +8486,18 @@
         <v>636.675</v>
       </c>
       <c r="M150" t="n">
+        <v>218.15</v>
+      </c>
+      <c r="N150" t="n">
+        <v>190213.75</v>
+      </c>
+      <c r="O150" t="n">
         <v>5449.225</v>
       </c>
-      <c r="N150" t="n">
-        <v>0</v>
-      </c>
-      <c r="O150" t="n">
+      <c r="P150" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q150" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7635,12 +8539,18 @@
         <v>644.525</v>
       </c>
       <c r="M151" t="n">
+        <v>157.35</v>
+      </c>
+      <c r="N151" t="n">
+        <v>189959.25</v>
+      </c>
+      <c r="O151" t="n">
         <v>5359.35</v>
       </c>
-      <c r="N151" t="n">
-        <v>0</v>
-      </c>
-      <c r="O151" t="n">
+      <c r="P151" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q151" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7682,12 +8592,18 @@
         <v>527.675</v>
       </c>
       <c r="M152" t="n">
+        <v>140.55</v>
+      </c>
+      <c r="N152" t="n">
+        <v>188156</v>
+      </c>
+      <c r="O152" t="n">
         <v>5280.45</v>
       </c>
-      <c r="N152" t="n">
-        <v>0</v>
-      </c>
-      <c r="O152" t="n">
+      <c r="P152" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q152" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7729,12 +8645,18 @@
         <v>581</v>
       </c>
       <c r="M153" t="n">
+        <v>142</v>
+      </c>
+      <c r="N153" t="n">
+        <v>190086.25</v>
+      </c>
+      <c r="O153" t="n">
         <v>5143.425</v>
       </c>
-      <c r="N153" t="n">
-        <v>0</v>
-      </c>
-      <c r="O153" t="n">
+      <c r="P153" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q153" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7776,12 +8698,18 @@
         <v>571.85</v>
       </c>
       <c r="M154" t="n">
+        <v>115.575</v>
+      </c>
+      <c r="N154" t="n">
+        <v>192217.25</v>
+      </c>
+      <c r="O154" t="n">
         <v>4985.849999999999</v>
       </c>
-      <c r="N154" t="n">
-        <v>0</v>
-      </c>
-      <c r="O154" t="n">
+      <c r="P154" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q154" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7823,12 +8751,18 @@
         <v>96</v>
       </c>
       <c r="M155" t="n">
+        <v>115.65</v>
+      </c>
+      <c r="N155" t="n">
+        <v>193078.25</v>
+      </c>
+      <c r="O155" t="n">
         <v>4365.5</v>
       </c>
-      <c r="N155" t="n">
-        <v>0</v>
-      </c>
-      <c r="O155" t="n">
+      <c r="P155" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q155" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7843,7 +8777,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8010,36 +8944,60 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Precipitación estimada acumulada últimos 60 días (mm)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Acumulado de precipitación estimada en los 60 días anteriores</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Radiación estimada acumulada últimos 60 días (Wh/m²)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Acumulado de radiación estimada en los 60 días anteriores</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>HDD acumulado últimos 60 días</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Acumulado de grados-día de calefacción en los 60 días anteriores</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Días con heladas (&lt; 4 °C)</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Cantidad de días con heladas (temperatura menor a 4 °C)</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Días con heladas (&lt; 4 °C)</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Cantidad de días con radiación solar registrada (mayor a 0 W/m²)</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Días soleados (Solar &gt; 0 W/m²)</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
-          <t>Acumulado de grados-día de calefacción en los 60 días anteriores</t>
+          <t>Cantidad de días con radiación solar registrada (mayor a 0 W/m²)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix:se da un mejor orden a las columnas en excel
</commit_message>
<xml_diff>
--- a/resumen_semanal_clima.xlsx
+++ b/resumen_semanal_clima.xlsx
@@ -572,22 +572,22 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>Precipitación estimada acumulada últimos 60 días (mm)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Radiación estimada (Wh/m²)</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Radiación estimada acumulada últimos 60 días (Wh/m²)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Grados-día calefacción (HDD)</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Precipitación estimada acumulada últimos 60 días (mm)</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Radiación estimada acumulada últimos 60 días (Wh/m²)</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -638,16 +638,16 @@
         <v>18.2</v>
       </c>
       <c r="K2" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="L2" t="n">
         <v>19635.5</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
+        <v>19635.5</v>
+      </c>
+      <c r="N2" t="n">
         <v>515.775</v>
-      </c>
-      <c r="M2" t="n">
-        <v>18.2</v>
-      </c>
-      <c r="N2" t="n">
-        <v>19635.5</v>
       </c>
       <c r="O2" t="n">
         <v>515.775</v>
@@ -691,16 +691,16 @@
         <v>31.1</v>
       </c>
       <c r="K3" t="n">
+        <v>49.3</v>
+      </c>
+      <c r="L3" t="n">
         <v>21904</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
+        <v>41539.5</v>
+      </c>
+      <c r="N3" t="n">
         <v>587.325</v>
-      </c>
-      <c r="M3" t="n">
-        <v>49.3</v>
-      </c>
-      <c r="N3" t="n">
-        <v>41539.5</v>
       </c>
       <c r="O3" t="n">
         <v>1103.1</v>
@@ -744,16 +744,16 @@
         <v>28.25</v>
       </c>
       <c r="K4" t="n">
+        <v>77.55</v>
+      </c>
+      <c r="L4" t="n">
         <v>20627.25</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
+        <v>62166.75</v>
+      </c>
+      <c r="N4" t="n">
         <v>555.525</v>
-      </c>
-      <c r="M4" t="n">
-        <v>77.55</v>
-      </c>
-      <c r="N4" t="n">
-        <v>62166.75</v>
       </c>
       <c r="O4" t="n">
         <v>1658.625</v>
@@ -797,16 +797,16 @@
         <v>36.05</v>
       </c>
       <c r="K5" t="n">
+        <v>113.6</v>
+      </c>
+      <c r="L5" t="n">
         <v>23172.5</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
+        <v>85339.25</v>
+      </c>
+      <c r="N5" t="n">
         <v>511.45</v>
-      </c>
-      <c r="M5" t="n">
-        <v>113.6</v>
-      </c>
-      <c r="N5" t="n">
-        <v>85339.25</v>
       </c>
       <c r="O5" t="n">
         <v>2170.075</v>
@@ -850,16 +850,16 @@
         <v>13.4</v>
       </c>
       <c r="K6" t="n">
+        <v>127</v>
+      </c>
+      <c r="L6" t="n">
         <v>29179.25</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
+        <v>114518.5</v>
+      </c>
+      <c r="N6" t="n">
         <v>533.5</v>
-      </c>
-      <c r="M6" t="n">
-        <v>127</v>
-      </c>
-      <c r="N6" t="n">
-        <v>114518.5</v>
       </c>
       <c r="O6" t="n">
         <v>2703.575</v>
@@ -903,16 +903,16 @@
         <v>12.875</v>
       </c>
       <c r="K7" t="n">
+        <v>139.875</v>
+      </c>
+      <c r="L7" t="n">
         <v>23801.25</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
+        <v>138319.75</v>
+      </c>
+      <c r="N7" t="n">
         <v>458.15</v>
-      </c>
-      <c r="M7" t="n">
-        <v>139.875</v>
-      </c>
-      <c r="N7" t="n">
-        <v>138319.75</v>
       </c>
       <c r="O7" t="n">
         <v>3161.725</v>
@@ -956,16 +956,16 @@
         <v>19</v>
       </c>
       <c r="K8" t="n">
+        <v>158.875</v>
+      </c>
+      <c r="L8" t="n">
         <v>21397.25</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
+        <v>159717</v>
+      </c>
+      <c r="N8" t="n">
         <v>539.025</v>
-      </c>
-      <c r="M8" t="n">
-        <v>158.875</v>
-      </c>
-      <c r="N8" t="n">
-        <v>159717</v>
       </c>
       <c r="O8" t="n">
         <v>3700.75</v>
@@ -1009,16 +1009,16 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
+        <v>158.875</v>
+      </c>
+      <c r="L9" t="n">
         <v>23386.25</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
+        <v>183103.25</v>
+      </c>
+      <c r="N9" t="n">
         <v>523.05</v>
-      </c>
-      <c r="M9" t="n">
-        <v>158.875</v>
-      </c>
-      <c r="N9" t="n">
-        <v>183103.25</v>
       </c>
       <c r="O9" t="n">
         <v>4223.8</v>
@@ -1062,16 +1062,16 @@
         <v>22.25</v>
       </c>
       <c r="K10" t="n">
+        <v>174.75</v>
+      </c>
+      <c r="L10" t="n">
         <v>24160.25</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
+        <v>198683.75</v>
+      </c>
+      <c r="N10" t="n">
         <v>515.5</v>
-      </c>
-      <c r="M10" t="n">
-        <v>174.75</v>
-      </c>
-      <c r="N10" t="n">
-        <v>198683.75</v>
       </c>
       <c r="O10" t="n">
         <v>4223.525</v>
@@ -1115,16 +1115,16 @@
         <v>46.35</v>
       </c>
       <c r="K11" t="n">
+        <v>196.7</v>
+      </c>
+      <c r="L11" t="n">
         <v>24816.25</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
+        <v>203377.5</v>
+      </c>
+      <c r="N11" t="n">
         <v>461.7</v>
-      </c>
-      <c r="M11" t="n">
-        <v>196.7</v>
-      </c>
-      <c r="N11" t="n">
-        <v>203377.5</v>
       </c>
       <c r="O11" t="n">
         <v>4097.9</v>
@@ -1168,16 +1168,16 @@
         <v>29.45</v>
       </c>
       <c r="K12" t="n">
+        <v>189.125</v>
+      </c>
+      <c r="L12" t="n">
         <v>27687.75</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
+        <v>208308</v>
+      </c>
+      <c r="N12" t="n">
         <v>565.275</v>
-      </c>
-      <c r="M12" t="n">
-        <v>189.125</v>
-      </c>
-      <c r="N12" t="n">
-        <v>208308</v>
       </c>
       <c r="O12" t="n">
         <v>4107.65</v>
@@ -1221,16 +1221,16 @@
         <v>23.8</v>
       </c>
       <c r="K13" t="n">
+        <v>201.75</v>
+      </c>
+      <c r="L13" t="n">
         <v>21734.5</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
+        <v>209152</v>
+      </c>
+      <c r="N13" t="n">
         <v>546.3</v>
-      </c>
-      <c r="M13" t="n">
-        <v>201.75</v>
-      </c>
-      <c r="N13" t="n">
-        <v>209152</v>
       </c>
       <c r="O13" t="n">
         <v>4142.5</v>
@@ -1274,16 +1274,16 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
+        <v>201.75</v>
+      </c>
+      <c r="L14" t="n">
         <v>3692.25</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
+        <v>209322.75</v>
+      </c>
+      <c r="N14" t="n">
         <v>80.3</v>
-      </c>
-      <c r="M14" t="n">
-        <v>201.75</v>
-      </c>
-      <c r="N14" t="n">
-        <v>209322.75</v>
       </c>
       <c r="O14" t="n">
         <v>3689.3</v>
@@ -1327,16 +1327,16 @@
         <v>15.225</v>
       </c>
       <c r="K15" t="n">
+        <v>182.35</v>
+      </c>
+      <c r="L15" t="n">
         <v>11074</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
+        <v>207287.25</v>
+      </c>
+      <c r="N15" t="n">
         <v>330.775</v>
-      </c>
-      <c r="M15" t="n">
-        <v>182.35</v>
-      </c>
-      <c r="N15" t="n">
-        <v>207287.25</v>
       </c>
       <c r="O15" t="n">
         <v>3561.925</v>
@@ -1380,16 +1380,16 @@
         <v>25.7</v>
       </c>
       <c r="K16" t="n">
+        <v>194.65</v>
+      </c>
+      <c r="L16" t="n">
         <v>20496.75</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
+        <v>199776.5</v>
+      </c>
+      <c r="N16" t="n">
         <v>514.575</v>
-      </c>
-      <c r="M16" t="n">
-        <v>194.65</v>
-      </c>
-      <c r="N16" t="n">
-        <v>199776.5</v>
       </c>
       <c r="O16" t="n">
         <v>3537.475</v>
@@ -1433,16 +1433,16 @@
         <v>15.525</v>
       </c>
       <c r="K17" t="n">
+        <v>194.075</v>
+      </c>
+      <c r="L17" t="n">
         <v>24663.25</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
+        <v>201090.25</v>
+      </c>
+      <c r="N17" t="n">
         <v>561.7</v>
-      </c>
-      <c r="M17" t="n">
-        <v>194.075</v>
-      </c>
-      <c r="N17" t="n">
-        <v>201090.25</v>
       </c>
       <c r="O17" t="n">
         <v>3576.125</v>
@@ -1486,16 +1486,16 @@
         <v>22.825</v>
       </c>
       <c r="K18" t="n">
+        <v>201.125</v>
+      </c>
+      <c r="L18" t="n">
         <v>25338.5</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
+        <v>203279.75</v>
+      </c>
+      <c r="N18" t="n">
         <v>619.4</v>
-      </c>
-      <c r="M18" t="n">
-        <v>201.125</v>
-      </c>
-      <c r="N18" t="n">
-        <v>203279.75</v>
       </c>
       <c r="O18" t="n">
         <v>3680.025</v>
@@ -1539,16 +1539,16 @@
         <v>30.2</v>
       </c>
       <c r="K19" t="n">
+        <v>229.025</v>
+      </c>
+      <c r="L19" t="n">
         <v>22924.75</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
+        <v>203041.5</v>
+      </c>
+      <c r="N19" t="n">
         <v>687.45</v>
-      </c>
-      <c r="M19" t="n">
-        <v>229.025</v>
-      </c>
-      <c r="N19" t="n">
-        <v>203041.5</v>
       </c>
       <c r="O19" t="n">
         <v>3905.775</v>
@@ -1592,16 +1592,16 @@
         <v>4.375</v>
       </c>
       <c r="K20" t="n">
+        <v>202.975</v>
+      </c>
+      <c r="L20" t="n">
         <v>27099</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
+        <v>205814.5</v>
+      </c>
+      <c r="N20" t="n">
         <v>605.575</v>
-      </c>
-      <c r="M20" t="n">
-        <v>202.975</v>
-      </c>
-      <c r="N20" t="n">
-        <v>205814.5</v>
       </c>
       <c r="O20" t="n">
         <v>3946.075</v>
@@ -1645,16 +1645,16 @@
         <v>16.55</v>
       </c>
       <c r="K21" t="n">
+        <v>183.65</v>
+      </c>
+      <c r="L21" t="n">
         <v>27346.25</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
+        <v>208282.75</v>
+      </c>
+      <c r="N21" t="n">
         <v>549.975</v>
-      </c>
-      <c r="M21" t="n">
-        <v>183.65</v>
-      </c>
-      <c r="N21" t="n">
-        <v>208282.75</v>
       </c>
       <c r="O21" t="n">
         <v>3949.75</v>
@@ -1698,16 +1698,16 @@
         <v>11.275</v>
       </c>
       <c r="K22" t="n">
+        <v>164.95</v>
+      </c>
+      <c r="L22" t="n">
         <v>21699.5</v>
       </c>
-      <c r="L22" t="n">
+      <c r="M22" t="n">
+        <v>203516.75</v>
+      </c>
+      <c r="N22" t="n">
         <v>523.775</v>
-      </c>
-      <c r="M22" t="n">
-        <v>164.95</v>
-      </c>
-      <c r="N22" t="n">
-        <v>203516.75</v>
       </c>
       <c r="O22" t="n">
         <v>4393.225</v>
@@ -1751,16 +1751,16 @@
         <v>10.7</v>
       </c>
       <c r="K23" t="n">
+        <v>152.375</v>
+      </c>
+      <c r="L23" t="n">
         <v>25005.75</v>
       </c>
-      <c r="L23" t="n">
+      <c r="M23" t="n">
+        <v>205647.75</v>
+      </c>
+      <c r="N23" t="n">
         <v>391.475</v>
-      </c>
-      <c r="M23" t="n">
-        <v>152.375</v>
-      </c>
-      <c r="N23" t="n">
-        <v>205647.75</v>
       </c>
       <c r="O23" t="n">
         <v>4453.925</v>
@@ -1804,16 +1804,16 @@
         <v>1.325</v>
       </c>
       <c r="K24" t="n">
+        <v>128.775</v>
+      </c>
+      <c r="L24" t="n">
         <v>34082.75</v>
       </c>
-      <c r="L24" t="n">
+      <c r="M24" t="n">
+        <v>224838.5</v>
+      </c>
+      <c r="N24" t="n">
         <v>537.125</v>
-      </c>
-      <c r="M24" t="n">
-        <v>128.775</v>
-      </c>
-      <c r="N24" t="n">
-        <v>224838.5</v>
       </c>
       <c r="O24" t="n">
         <v>4476.475</v>
@@ -1857,16 +1857,16 @@
         <v>1.4</v>
       </c>
       <c r="K25" t="n">
+        <v>108.825</v>
+      </c>
+      <c r="L25" t="n">
         <v>29612.75</v>
       </c>
-      <c r="L25" t="n">
+      <c r="M25" t="n">
+        <v>225918.75</v>
+      </c>
+      <c r="N25" t="n">
         <v>546.525</v>
-      </c>
-      <c r="M25" t="n">
-        <v>108.825</v>
-      </c>
-      <c r="N25" t="n">
-        <v>225918.75</v>
       </c>
       <c r="O25" t="n">
         <v>4461.3</v>
@@ -1910,16 +1910,16 @@
         <v>13.25</v>
       </c>
       <c r="K26" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="L26" t="n">
         <v>22297.75</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
+        <v>223642</v>
+      </c>
+      <c r="N26" t="n">
         <v>615.7</v>
-      </c>
-      <c r="M26" t="n">
-        <v>95.3</v>
-      </c>
-      <c r="N26" t="n">
-        <v>223642</v>
       </c>
       <c r="O26" t="n">
         <v>4457.6</v>
@@ -1963,16 +1963,16 @@
         <v>53.55</v>
       </c>
       <c r="K27" t="n">
+        <v>136.4</v>
+      </c>
+      <c r="L27" t="n">
         <v>23111.75</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
+        <v>222562.25</v>
+      </c>
+      <c r="N27" t="n">
         <v>615.3</v>
-      </c>
-      <c r="M27" t="n">
-        <v>136.4</v>
-      </c>
-      <c r="N27" t="n">
-        <v>222562.25</v>
       </c>
       <c r="O27" t="n">
         <v>4385.45</v>
@@ -2016,16 +2016,16 @@
         <v>35.85</v>
       </c>
       <c r="K28" t="n">
+        <v>147.4</v>
+      </c>
+      <c r="L28" t="n">
         <v>19157.5</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
+        <v>215723.25</v>
+      </c>
+      <c r="N28" t="n">
         <v>346.8</v>
-      </c>
-      <c r="M28" t="n">
-        <v>147.4</v>
-      </c>
-      <c r="N28" t="n">
-        <v>215723.25</v>
       </c>
       <c r="O28" t="n">
         <v>4126.675</v>
@@ -2069,16 +2069,16 @@
         <v>0</v>
       </c>
       <c r="K29" t="n">
+        <v>127.65</v>
+      </c>
+      <c r="L29" t="n">
         <v>30840.5</v>
       </c>
-      <c r="L29" t="n">
+      <c r="M29" t="n">
+        <v>222985.5</v>
+      </c>
+      <c r="N29" t="n">
         <v>448.25</v>
-      </c>
-      <c r="M29" t="n">
-        <v>127.65</v>
-      </c>
-      <c r="N29" t="n">
-        <v>222985.5</v>
       </c>
       <c r="O29" t="n">
         <v>4024.95</v>
@@ -2122,16 +2122,16 @@
         <v>0</v>
       </c>
       <c r="K30" t="n">
+        <v>116.075</v>
+      </c>
+      <c r="L30" t="n">
         <v>34203</v>
       </c>
-      <c r="L30" t="n">
+      <c r="M30" t="n">
+        <v>232420.75</v>
+      </c>
+      <c r="N30" t="n">
         <v>413.35</v>
-      </c>
-      <c r="M30" t="n">
-        <v>116.075</v>
-      </c>
-      <c r="N30" t="n">
-        <v>232420.75</v>
       </c>
       <c r="O30" t="n">
         <v>3914.525</v>
@@ -2175,16 +2175,16 @@
         <v>5.324999999999999</v>
       </c>
       <c r="K31" t="n">
+        <v>120.55</v>
+      </c>
+      <c r="L31" t="n">
         <v>29999.5</v>
       </c>
-      <c r="L31" t="n">
+      <c r="M31" t="n">
+        <v>239291</v>
+      </c>
+      <c r="N31" t="n">
         <v>618.95</v>
-      </c>
-      <c r="M31" t="n">
-        <v>120.55</v>
-      </c>
-      <c r="N31" t="n">
-        <v>239291</v>
       </c>
       <c r="O31" t="n">
         <v>4142</v>
@@ -2228,16 +2228,16 @@
         <v>24.85</v>
       </c>
       <c r="K32" t="n">
+        <v>134.525</v>
+      </c>
+      <c r="L32" t="n">
         <v>25896.75</v>
       </c>
-      <c r="L32" t="n">
+      <c r="M32" t="n">
+        <v>234154.75</v>
+      </c>
+      <c r="N32" t="n">
         <v>598.825</v>
-      </c>
-      <c r="M32" t="n">
-        <v>134.525</v>
-      </c>
-      <c r="N32" t="n">
-        <v>234154.75</v>
       </c>
       <c r="O32" t="n">
         <v>4203.700000000001</v>
@@ -2281,16 +2281,16 @@
         <v>18.55</v>
       </c>
       <c r="K33" t="n">
+        <v>152.775</v>
+      </c>
+      <c r="L33" t="n">
         <v>31963.5</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M33" t="n">
+        <v>232150.5</v>
+      </c>
+      <c r="N33" t="n">
         <v>558.45</v>
-      </c>
-      <c r="M33" t="n">
-        <v>152.775</v>
-      </c>
-      <c r="N33" t="n">
-        <v>232150.5</v>
       </c>
       <c r="O33" t="n">
         <v>4215.625</v>
@@ -2334,16 +2334,16 @@
         <v>1.625</v>
       </c>
       <c r="K34" t="n">
+        <v>150.7</v>
+      </c>
+      <c r="L34" t="n">
         <v>20294.75</v>
       </c>
-      <c r="L34" t="n">
+      <c r="M34" t="n">
+        <v>229593.75</v>
+      </c>
+      <c r="N34" t="n">
         <v>669.175</v>
-      </c>
-      <c r="M34" t="n">
-        <v>150.7</v>
-      </c>
-      <c r="N34" t="n">
-        <v>229593.75</v>
       </c>
       <c r="O34" t="n">
         <v>4269.1</v>
@@ -2387,16 +2387,16 @@
         <v>3.1</v>
       </c>
       <c r="K35" t="n">
+        <v>151.725</v>
+      </c>
+      <c r="L35" t="n">
         <v>5376</v>
       </c>
-      <c r="L35" t="n">
+      <c r="M35" t="n">
+        <v>224954.25</v>
+      </c>
+      <c r="N35" t="n">
         <v>131.2</v>
-      </c>
-      <c r="M35" t="n">
-        <v>151.725</v>
-      </c>
-      <c r="N35" t="n">
-        <v>224954.25</v>
       </c>
       <c r="O35" t="n">
         <v>3785</v>
@@ -2440,16 +2440,16 @@
         <v>8.699999999999999</v>
       </c>
       <c r="K36" t="n">
+        <v>105.725</v>
+      </c>
+      <c r="L36" t="n">
         <v>25198.5</v>
       </c>
-      <c r="L36" t="n">
+      <c r="M36" t="n">
+        <v>232047.75</v>
+      </c>
+      <c r="N36" t="n">
         <v>555.45</v>
-      </c>
-      <c r="M36" t="n">
-        <v>105.725</v>
-      </c>
-      <c r="N36" t="n">
-        <v>232047.75</v>
       </c>
       <c r="O36" t="n">
         <v>3993.65</v>
@@ -2493,16 +2493,16 @@
         <v>0</v>
       </c>
       <c r="K37" t="n">
+        <v>70.64999999999999</v>
+      </c>
+      <c r="L37" t="n">
         <v>20898.25</v>
       </c>
-      <c r="L37" t="n">
+      <c r="M37" t="n">
+        <v>231800.5</v>
+      </c>
+      <c r="N37" t="n">
         <v>352.4</v>
-      </c>
-      <c r="M37" t="n">
-        <v>70.64999999999999</v>
-      </c>
-      <c r="N37" t="n">
-        <v>231800.5</v>
       </c>
       <c r="O37" t="n">
         <v>3897.8</v>
@@ -2546,16 +2546,16 @@
         <v>5.05</v>
       </c>
       <c r="K38" t="n">
+        <v>67.19999999999999</v>
+      </c>
+      <c r="L38" t="n">
         <v>23232.75</v>
       </c>
-      <c r="L38" t="n">
+      <c r="M38" t="n">
+        <v>238876</v>
+      </c>
+      <c r="N38" t="n">
         <v>694.6</v>
-      </c>
-      <c r="M38" t="n">
-        <v>67.19999999999999</v>
-      </c>
-      <c r="N38" t="n">
-        <v>238876</v>
       </c>
       <c r="O38" t="n">
         <v>4179.05</v>
@@ -2599,16 +2599,16 @@
         <v>15.25</v>
       </c>
       <c r="K39" t="n">
+        <v>82.44999999999999</v>
+      </c>
+      <c r="L39" t="n">
         <v>26927.25</v>
       </c>
-      <c r="L39" t="n">
+      <c r="M39" t="n">
+        <v>228827.75</v>
+      </c>
+      <c r="N39" t="n">
         <v>699.325</v>
-      </c>
-      <c r="M39" t="n">
-        <v>82.44999999999999</v>
-      </c>
-      <c r="N39" t="n">
-        <v>228827.75</v>
       </c>
       <c r="O39" t="n">
         <v>4259.425</v>
@@ -2652,16 +2652,16 @@
         <v>0.825</v>
       </c>
       <c r="K40" t="n">
+        <v>83.27499999999999</v>
+      </c>
+      <c r="L40" t="n">
         <v>9531.5</v>
       </c>
-      <c r="L40" t="n">
+      <c r="M40" t="n">
+        <v>219318.75</v>
+      </c>
+      <c r="N40" t="n">
         <v>305.725</v>
-      </c>
-      <c r="M40" t="n">
-        <v>83.27499999999999</v>
-      </c>
-      <c r="N40" t="n">
-        <v>219318.75</v>
       </c>
       <c r="O40" t="n">
         <v>3966.325</v>
@@ -2705,16 +2705,16 @@
         <v>41.95</v>
       </c>
       <c r="K41" t="n">
+        <v>119.9</v>
+      </c>
+      <c r="L41" t="n">
         <v>24627.75</v>
       </c>
-      <c r="L41" t="n">
+      <c r="M41" t="n">
+        <v>213947</v>
+      </c>
+      <c r="N41" t="n">
         <v>665.075</v>
-      </c>
-      <c r="M41" t="n">
-        <v>119.9</v>
-      </c>
-      <c r="N41" t="n">
-        <v>213947</v>
       </c>
       <c r="O41" t="n">
         <v>4072.95</v>
@@ -2758,16 +2758,16 @@
         <v>16.85</v>
       </c>
       <c r="K42" t="n">
+        <v>111.9</v>
+      </c>
+      <c r="L42" t="n">
         <v>21309.25</v>
       </c>
-      <c r="L42" t="n">
+      <c r="M42" t="n">
+        <v>209359.5</v>
+      </c>
+      <c r="N42" t="n">
         <v>682.85</v>
-      </c>
-      <c r="M42" t="n">
-        <v>111.9</v>
-      </c>
-      <c r="N42" t="n">
-        <v>209359.5</v>
       </c>
       <c r="O42" t="n">
         <v>4086.625</v>
@@ -2811,16 +2811,16 @@
         <v>0.5</v>
       </c>
       <c r="K43" t="n">
+        <v>93.84999999999999</v>
+      </c>
+      <c r="L43" t="n">
         <v>29659.25</v>
       </c>
-      <c r="L43" t="n">
+      <c r="M43" t="n">
+        <v>207055.25</v>
+      </c>
+      <c r="N43" t="n">
         <v>640.35</v>
-      </c>
-      <c r="M43" t="n">
-        <v>93.84999999999999</v>
-      </c>
-      <c r="N43" t="n">
-        <v>207055.25</v>
       </c>
       <c r="O43" t="n">
         <v>4595.775000000001</v>
@@ -2864,16 +2864,16 @@
         <v>0</v>
       </c>
       <c r="K44" t="n">
+        <v>92.22499999999999</v>
+      </c>
+      <c r="L44" t="n">
         <v>23087.75</v>
       </c>
-      <c r="L44" t="n">
+      <c r="M44" t="n">
+        <v>207628.5</v>
+      </c>
+      <c r="N44" t="n">
         <v>773.95</v>
-      </c>
-      <c r="M44" t="n">
-        <v>92.22499999999999</v>
-      </c>
-      <c r="N44" t="n">
-        <v>207628.5</v>
       </c>
       <c r="O44" t="n">
         <v>4814.275000000001</v>
@@ -2917,16 +2917,16 @@
         <v>0.6</v>
       </c>
       <c r="K45" t="n">
+        <v>81.02500000000001</v>
+      </c>
+      <c r="L45" t="n">
         <v>23243.75</v>
       </c>
-      <c r="L45" t="n">
+      <c r="M45" t="n">
+        <v>210802</v>
+      </c>
+      <c r="N45" t="n">
         <v>841.875</v>
-      </c>
-      <c r="M45" t="n">
-        <v>81.02500000000001</v>
-      </c>
-      <c r="N45" t="n">
-        <v>210802</v>
       </c>
       <c r="O45" t="n">
         <v>5303.750000000001</v>
@@ -2970,16 +2970,16 @@
         <v>35.1</v>
       </c>
       <c r="K46" t="n">
+        <v>116.125</v>
+      </c>
+      <c r="L46" t="n">
         <v>18369.5</v>
       </c>
-      <c r="L46" t="n">
+      <c r="M46" t="n">
+        <v>199988.75</v>
+      </c>
+      <c r="N46" t="n">
         <v>734.475</v>
-      </c>
-      <c r="M46" t="n">
-        <v>116.125</v>
-      </c>
-      <c r="N46" t="n">
-        <v>199988.75</v>
       </c>
       <c r="O46" t="n">
         <v>5343.625</v>
@@ -3023,16 +3023,16 @@
         <v>11.175</v>
       </c>
       <c r="K47" t="n">
+        <v>122.25</v>
+      </c>
+      <c r="L47" t="n">
         <v>22894.75</v>
       </c>
-      <c r="L47" t="n">
+      <c r="M47" t="n">
+        <v>199650.75</v>
+      </c>
+      <c r="N47" t="n">
         <v>717.3</v>
-      </c>
-      <c r="M47" t="n">
-        <v>122.25</v>
-      </c>
-      <c r="N47" t="n">
-        <v>199650.75</v>
       </c>
       <c r="O47" t="n">
         <v>5361.6</v>
@@ -3076,16 +3076,16 @@
         <v>21.6</v>
       </c>
       <c r="K48" t="n">
+        <v>128.6</v>
+      </c>
+      <c r="L48" t="n">
         <v>25120</v>
       </c>
-      <c r="L48" t="n">
+      <c r="M48" t="n">
+        <v>197843.5</v>
+      </c>
+      <c r="N48" t="n">
         <v>679.45</v>
-      </c>
-      <c r="M48" t="n">
-        <v>128.6</v>
-      </c>
-      <c r="N48" t="n">
-        <v>197843.5</v>
       </c>
       <c r="O48" t="n">
         <v>5735.325</v>
@@ -3129,16 +3129,16 @@
         <v>2.6</v>
       </c>
       <c r="K49" t="n">
+        <v>123.85</v>
+      </c>
+      <c r="L49" t="n">
         <v>21130.25</v>
       </c>
-      <c r="L49" t="n">
+      <c r="M49" t="n">
+        <v>196727.75</v>
+      </c>
+      <c r="N49" t="n">
         <v>617.25</v>
-      </c>
-      <c r="M49" t="n">
-        <v>123.85</v>
-      </c>
-      <c r="N49" t="n">
-        <v>196727.75</v>
       </c>
       <c r="O49" t="n">
         <v>5687.5</v>
@@ -3182,16 +3182,16 @@
         <v>22.05</v>
       </c>
       <c r="K50" t="n">
+        <v>102.025</v>
+      </c>
+      <c r="L50" t="n">
         <v>23987.25</v>
       </c>
-      <c r="L50" t="n">
+      <c r="M50" t="n">
+        <v>200216</v>
+      </c>
+      <c r="N50" t="n">
         <v>810.025</v>
-      </c>
-      <c r="M50" t="n">
-        <v>102.025</v>
-      </c>
-      <c r="N50" t="n">
-        <v>200216</v>
       </c>
       <c r="O50" t="n">
         <v>5814.675</v>
@@ -3235,16 +3235,16 @@
         <v>7.925</v>
       </c>
       <c r="K51" t="n">
+        <v>101.05</v>
+      </c>
+      <c r="L51" t="n">
         <v>24427.5</v>
       </c>
-      <c r="L51" t="n">
+      <c r="M51" t="n">
+        <v>199370.25</v>
+      </c>
+      <c r="N51" t="n">
         <v>766.2</v>
-      </c>
-      <c r="M51" t="n">
-        <v>101.05</v>
-      </c>
-      <c r="N51" t="n">
-        <v>199370.25</v>
       </c>
       <c r="O51" t="n">
         <v>5940.525000000001</v>
@@ -3288,16 +3288,16 @@
         <v>30.95</v>
       </c>
       <c r="K52" t="n">
+        <v>132</v>
+      </c>
+      <c r="L52" t="n">
         <v>19751.5</v>
       </c>
-      <c r="L52" t="n">
+      <c r="M52" t="n">
+        <v>193086</v>
+      </c>
+      <c r="N52" t="n">
         <v>611.95</v>
-      </c>
-      <c r="M52" t="n">
-        <v>132</v>
-      </c>
-      <c r="N52" t="n">
-        <v>193086</v>
       </c>
       <c r="O52" t="n">
         <v>5778.525</v>
@@ -3341,16 +3341,16 @@
         <v>10.325</v>
       </c>
       <c r="K53" t="n">
+        <v>141.725</v>
+      </c>
+      <c r="L53" t="n">
         <v>22262.5</v>
       </c>
-      <c r="L53" t="n">
+      <c r="M53" t="n">
+        <v>191337.25</v>
+      </c>
+      <c r="N53" t="n">
         <v>657.5</v>
-      </c>
-      <c r="M53" t="n">
-        <v>141.725</v>
-      </c>
-      <c r="N53" t="n">
-        <v>191337.25</v>
       </c>
       <c r="O53" t="n">
         <v>5594.15</v>
@@ -3392,16 +3392,16 @@
         <v>0.8999999999999999</v>
       </c>
       <c r="K54" t="n">
+        <v>133.75</v>
+      </c>
+      <c r="L54" t="n">
         <v>19903.25</v>
       </c>
-      <c r="L54" t="n">
+      <c r="M54" t="n">
+        <v>190323.75</v>
+      </c>
+      <c r="N54" t="n">
         <v>666.225</v>
-      </c>
-      <c r="M54" t="n">
-        <v>133.75</v>
-      </c>
-      <c r="N54" t="n">
-        <v>190323.75</v>
       </c>
       <c r="O54" t="n">
         <v>5525.900000000001</v>
@@ -3445,16 +3445,16 @@
         <v>31.775</v>
       </c>
       <c r="K55" t="n">
+        <v>129.275</v>
+      </c>
+      <c r="L55" t="n">
         <v>22319.25</v>
       </c>
-      <c r="L55" t="n">
+      <c r="M55" t="n">
+        <v>192076.75</v>
+      </c>
+      <c r="N55" t="n">
         <v>776.75</v>
-      </c>
-      <c r="M55" t="n">
-        <v>129.275</v>
-      </c>
-      <c r="N55" t="n">
-        <v>192076.75</v>
       </c>
       <c r="O55" t="n">
         <v>5585.35</v>
@@ -3498,16 +3498,16 @@
         <v>9.15</v>
       </c>
       <c r="K56" t="n">
+        <v>118.075</v>
+      </c>
+      <c r="L56" t="n">
         <v>22961.75</v>
       </c>
-      <c r="L56" t="n">
+      <c r="M56" t="n">
+        <v>190882.75</v>
+      </c>
+      <c r="N56" t="n">
         <v>633.9</v>
-      </c>
-      <c r="M56" t="n">
-        <v>118.075</v>
-      </c>
-      <c r="N56" t="n">
-        <v>190882.75</v>
       </c>
       <c r="O56" t="n">
         <v>5539.8</v>
@@ -3551,16 +3551,16 @@
         <v>6.075</v>
       </c>
       <c r="K57" t="n">
+        <v>119.95</v>
+      </c>
+      <c r="L57" t="n">
         <v>23795</v>
       </c>
-      <c r="L57" t="n">
+      <c r="M57" t="n">
+        <v>191397.5</v>
+      </c>
+      <c r="N57" t="n">
         <v>610.575</v>
-      </c>
-      <c r="M57" t="n">
-        <v>119.95</v>
-      </c>
-      <c r="N57" t="n">
-        <v>191397.5</v>
       </c>
       <c r="O57" t="n">
         <v>5533.125</v>
@@ -3604,16 +3604,16 @@
         <v>31.625</v>
       </c>
       <c r="K58" t="n">
+        <v>150.775</v>
+      </c>
+      <c r="L58" t="n">
         <v>23835</v>
       </c>
-      <c r="L58" t="n">
+      <c r="M58" t="n">
+        <v>192559.5</v>
+      </c>
+      <c r="N58" t="n">
         <v>742.675</v>
-      </c>
-      <c r="M58" t="n">
-        <v>150.775</v>
-      </c>
-      <c r="N58" t="n">
-        <v>192559.5</v>
       </c>
       <c r="O58" t="n">
         <v>5465.775</v>
@@ -3657,16 +3657,16 @@
         <v>23.55</v>
       </c>
       <c r="K59" t="n">
+        <v>151.675</v>
+      </c>
+      <c r="L59" t="n">
         <v>30648.25</v>
       </c>
-      <c r="L59" t="n">
+      <c r="M59" t="n">
+        <v>199419.5</v>
+      </c>
+      <c r="N59" t="n">
         <v>705.7</v>
-      </c>
-      <c r="M59" t="n">
-        <v>151.675</v>
-      </c>
-      <c r="N59" t="n">
-        <v>199419.5</v>
       </c>
       <c r="O59" t="n">
         <v>5405.275</v>
@@ -3710,16 +3710,16 @@
         <v>0.3</v>
       </c>
       <c r="K60" t="n">
+        <v>134.55</v>
+      </c>
+      <c r="L60" t="n">
         <v>30533.75</v>
       </c>
-      <c r="L60" t="n">
+      <c r="M60" t="n">
+        <v>207409.75</v>
+      </c>
+      <c r="N60" t="n">
         <v>704.625</v>
-      </c>
-      <c r="M60" t="n">
-        <v>134.55</v>
-      </c>
-      <c r="N60" t="n">
-        <v>207409.75</v>
       </c>
       <c r="O60" t="n">
         <v>5497.95</v>
@@ -3763,16 +3763,16 @@
         <v>5.45</v>
       </c>
       <c r="K61" t="n">
+        <v>118.25</v>
+      </c>
+      <c r="L61" t="n">
         <v>23733.75</v>
       </c>
-      <c r="L61" t="n">
+      <c r="M61" t="n">
+        <v>211909.75</v>
+      </c>
+      <c r="N61" t="n">
         <v>611.975</v>
-      </c>
-      <c r="M61" t="n">
-        <v>118.25</v>
-      </c>
-      <c r="N61" t="n">
-        <v>211909.75</v>
       </c>
       <c r="O61" t="n">
         <v>5452.425</v>
@@ -3816,16 +3816,16 @@
         <v>0.95</v>
       </c>
       <c r="K62" t="n">
+        <v>108.875</v>
+      </c>
+      <c r="L62" t="n">
         <v>27422.5</v>
       </c>
-      <c r="L62" t="n">
+      <c r="M62" t="n">
+        <v>217441.25</v>
+      </c>
+      <c r="N62" t="n">
         <v>601.85</v>
-      </c>
-      <c r="M62" t="n">
-        <v>108.875</v>
-      </c>
-      <c r="N62" t="n">
-        <v>217441.25</v>
       </c>
       <c r="O62" t="n">
         <v>5388.05</v>
@@ -3869,16 +3869,16 @@
         <v>21.725</v>
       </c>
       <c r="K63" t="n">
+        <v>106.075</v>
+      </c>
+      <c r="L63" t="n">
         <v>27417.25</v>
       </c>
-      <c r="L63" t="n">
+      <c r="M63" t="n">
+        <v>222838</v>
+      </c>
+      <c r="N63" t="n">
         <v>582.375</v>
-      </c>
-      <c r="M63" t="n">
-        <v>106.075</v>
-      </c>
-      <c r="N63" t="n">
-        <v>222838</v>
       </c>
       <c r="O63" t="n">
         <v>5193.675</v>
@@ -3922,16 +3922,16 @@
         <v>8.475</v>
       </c>
       <c r="K64" t="n">
+        <v>103.3</v>
+      </c>
+      <c r="L64" t="n">
         <v>29749.5</v>
       </c>
-      <c r="L64" t="n">
+      <c r="M64" t="n">
+        <v>231075.25</v>
+      </c>
+      <c r="N64" t="n">
         <v>718.65</v>
-      </c>
-      <c r="M64" t="n">
-        <v>103.3</v>
-      </c>
-      <c r="N64" t="n">
-        <v>231075.25</v>
       </c>
       <c r="O64" t="n">
         <v>5278.425</v>
@@ -3975,16 +3975,16 @@
         <v>28.975</v>
       </c>
       <c r="K65" t="n">
+        <v>126.825</v>
+      </c>
+      <c r="L65" t="n">
         <v>26251.5</v>
       </c>
-      <c r="L65" t="n">
+      <c r="M65" t="n">
+        <v>232812</v>
+      </c>
+      <c r="N65" t="n">
         <v>745.875</v>
-      </c>
-      <c r="M65" t="n">
-        <v>126.825</v>
-      </c>
-      <c r="N65" t="n">
-        <v>232812</v>
       </c>
       <c r="O65" t="n">
         <v>5413.725</v>
@@ -4028,16 +4028,16 @@
         <v>18.375</v>
       </c>
       <c r="K66" t="n">
+        <v>132.8</v>
+      </c>
+      <c r="L66" t="n">
         <v>27903.25</v>
       </c>
-      <c r="L66" t="n">
+      <c r="M66" t="n">
+        <v>237389</v>
+      </c>
+      <c r="N66" t="n">
         <v>803.9</v>
-      </c>
-      <c r="M66" t="n">
-        <v>132.8</v>
-      </c>
-      <c r="N66" t="n">
-        <v>237389</v>
       </c>
       <c r="O66" t="n">
         <v>5474.95</v>
@@ -4081,16 +4081,16 @@
         <v>15.7</v>
       </c>
       <c r="K67" t="n">
+        <v>100.25</v>
+      </c>
+      <c r="L67" t="n">
         <v>23206.25</v>
       </c>
-      <c r="L67" t="n">
+      <c r="M67" t="n">
+        <v>234887.25</v>
+      </c>
+      <c r="N67" t="n">
         <v>656.25</v>
-      </c>
-      <c r="M67" t="n">
-        <v>100.25</v>
-      </c>
-      <c r="N67" t="n">
-        <v>234887.25</v>
       </c>
       <c r="O67" t="n">
         <v>5425.5</v>
@@ -4134,16 +4134,16 @@
         <v>57.1</v>
       </c>
       <c r="K68" t="n">
+        <v>157.05</v>
+      </c>
+      <c r="L68" t="n">
         <v>26973.5</v>
       </c>
-      <c r="L68" t="n">
+      <c r="M68" t="n">
+        <v>229690.75</v>
+      </c>
+      <c r="N68" t="n">
         <v>739.025</v>
-      </c>
-      <c r="M68" t="n">
-        <v>157.05</v>
-      </c>
-      <c r="N68" t="n">
-        <v>229690.75</v>
       </c>
       <c r="O68" t="n">
         <v>5459.900000000001</v>
@@ -4187,16 +4187,16 @@
         <v>31.5</v>
       </c>
       <c r="K69" t="n">
+        <v>188.25</v>
+      </c>
+      <c r="L69" t="n">
         <v>20598.25</v>
       </c>
-      <c r="L69" t="n">
+      <c r="M69" t="n">
+        <v>220164.75</v>
+      </c>
+      <c r="N69" t="n">
         <v>749.925</v>
-      </c>
-      <c r="M69" t="n">
-        <v>188.25</v>
-      </c>
-      <c r="N69" t="n">
-        <v>220164.75</v>
       </c>
       <c r="O69" t="n">
         <v>5597.85</v>
@@ -4240,16 +4240,16 @@
         <v>8.125</v>
       </c>
       <c r="K70" t="n">
+        <v>190.475</v>
+      </c>
+      <c r="L70" t="n">
         <v>23340.5</v>
       </c>
-      <c r="L70" t="n">
+      <c r="M70" t="n">
+        <v>218533.5</v>
+      </c>
+      <c r="N70" t="n">
         <v>855.35</v>
-      </c>
-      <c r="M70" t="n">
-        <v>190.475</v>
-      </c>
-      <c r="N70" t="n">
-        <v>218533.5</v>
       </c>
       <c r="O70" t="n">
         <v>5851.349999999999</v>
@@ -4293,16 +4293,16 @@
         <v>11.4</v>
       </c>
       <c r="K71" t="n">
+        <v>201.375</v>
+      </c>
+      <c r="L71" t="n">
         <v>29330.25</v>
       </c>
-      <c r="L71" t="n">
+      <c r="M71" t="n">
+        <v>226476.5</v>
+      </c>
+      <c r="N71" t="n">
         <v>872.2</v>
-      </c>
-      <c r="M71" t="n">
-        <v>201.375</v>
-      </c>
-      <c r="N71" t="n">
-        <v>226476.5</v>
       </c>
       <c r="O71" t="n">
         <v>6141.174999999999</v>
@@ -4346,16 +4346,16 @@
         <v>1.4</v>
       </c>
       <c r="K72" t="n">
+        <v>177.575</v>
+      </c>
+      <c r="L72" t="n">
         <v>29024.5</v>
       </c>
-      <c r="L72" t="n">
+      <c r="M72" t="n">
+        <v>223833.5</v>
+      </c>
+      <c r="N72" t="n">
         <v>674.525</v>
-      </c>
-      <c r="M72" t="n">
-        <v>177.575</v>
-      </c>
-      <c r="N72" t="n">
-        <v>223833.5</v>
       </c>
       <c r="O72" t="n">
         <v>6097.05</v>
@@ -4399,16 +4399,16 @@
         <v>0.3</v>
       </c>
       <c r="K73" t="n">
+        <v>167.2</v>
+      </c>
+      <c r="L73" t="n">
         <v>31002.25</v>
       </c>
-      <c r="L73" t="n">
+      <c r="M73" t="n">
+        <v>225631</v>
+      </c>
+      <c r="N73" t="n">
         <v>624.375</v>
-      </c>
-      <c r="M73" t="n">
-        <v>167.2</v>
-      </c>
-      <c r="N73" t="n">
-        <v>225631</v>
       </c>
       <c r="O73" t="n">
         <v>5975.55</v>
@@ -4452,16 +4452,16 @@
         <v>4.95</v>
       </c>
       <c r="K74" t="n">
+        <v>130.975</v>
+      </c>
+      <c r="L74" t="n">
         <v>26969</v>
       </c>
-      <c r="L74" t="n">
+      <c r="M74" t="n">
+        <v>226517.75</v>
+      </c>
+      <c r="N74" t="n">
         <v>596.95</v>
-      </c>
-      <c r="M74" t="n">
-        <v>130.975</v>
-      </c>
-      <c r="N74" t="n">
-        <v>226517.75</v>
       </c>
       <c r="O74" t="n">
         <v>5768.6</v>
@@ -4505,16 +4505,16 @@
         <v>14.9</v>
       </c>
       <c r="K75" t="n">
+        <v>129.675</v>
+      </c>
+      <c r="L75" t="n">
         <v>24474</v>
       </c>
-      <c r="L75" t="n">
+      <c r="M75" t="n">
+        <v>224364</v>
+      </c>
+      <c r="N75" t="n">
         <v>797.775</v>
-      </c>
-      <c r="M75" t="n">
-        <v>129.675</v>
-      </c>
-      <c r="N75" t="n">
-        <v>224364</v>
       </c>
       <c r="O75" t="n">
         <v>5910.125</v>
@@ -4558,16 +4558,16 @@
         <v>12.275</v>
       </c>
       <c r="K76" t="n">
+        <v>117.825</v>
+      </c>
+      <c r="L76" t="n">
         <v>26981.75</v>
       </c>
-      <c r="L76" t="n">
+      <c r="M76" t="n">
+        <v>225983.5</v>
+      </c>
+      <c r="N76" t="n">
         <v>820.575</v>
-      </c>
-      <c r="M76" t="n">
-        <v>117.825</v>
-      </c>
-      <c r="N76" t="n">
-        <v>225983.5</v>
       </c>
       <c r="O76" t="n">
         <v>5991.675</v>
@@ -4611,16 +4611,16 @@
         <v>13.55</v>
       </c>
       <c r="K77" t="n">
+        <v>94.27499999999999</v>
+      </c>
+      <c r="L77" t="n">
         <v>24526.25</v>
       </c>
-      <c r="L77" t="n">
+      <c r="M77" t="n">
+        <v>226335.25</v>
+      </c>
+      <c r="N77" t="n">
         <v>863.15</v>
-      </c>
-      <c r="M77" t="n">
-        <v>94.27499999999999</v>
-      </c>
-      <c r="N77" t="n">
-        <v>226335.25</v>
       </c>
       <c r="O77" t="n">
         <v>6104.9</v>
@@ -4664,16 +4664,16 @@
         <v>0</v>
       </c>
       <c r="K78" t="n">
+        <v>59.075</v>
+      </c>
+      <c r="L78" t="n">
         <v>36223.25</v>
       </c>
-      <c r="L78" t="n">
+      <c r="M78" t="n">
+        <v>242668</v>
+      </c>
+      <c r="N78" t="n">
         <v>718.375</v>
-      </c>
-      <c r="M78" t="n">
-        <v>59.075</v>
-      </c>
-      <c r="N78" t="n">
-        <v>242668</v>
       </c>
       <c r="O78" t="n">
         <v>5967.925</v>
@@ -4717,16 +4717,16 @@
         <v>8.025</v>
       </c>
       <c r="K79" t="n">
+        <v>64.8</v>
+      </c>
+      <c r="L79" t="n">
         <v>35551.5</v>
       </c>
-      <c r="L79" t="n">
+      <c r="M79" t="n">
+        <v>252542.5</v>
+      </c>
+      <c r="N79" t="n">
         <v>688.975</v>
-      </c>
-      <c r="M79" t="n">
-        <v>64.8</v>
-      </c>
-      <c r="N79" t="n">
-        <v>252542.5</v>
       </c>
       <c r="O79" t="n">
         <v>5784.700000000001</v>
@@ -4770,16 +4770,16 @@
         <v>0</v>
       </c>
       <c r="K80" t="n">
+        <v>54</v>
+      </c>
+      <c r="L80" t="n">
         <v>33464.75</v>
       </c>
-      <c r="L80" t="n">
+      <c r="M80" t="n">
+        <v>254270.75</v>
+      </c>
+      <c r="N80" t="n">
         <v>655.2</v>
-      </c>
-      <c r="M80" t="n">
-        <v>54</v>
-      </c>
-      <c r="N80" t="n">
-        <v>254270.75</v>
       </c>
       <c r="O80" t="n">
         <v>5765.375</v>
@@ -4823,16 +4823,16 @@
         <v>0</v>
       </c>
       <c r="K81" t="n">
+        <v>54</v>
+      </c>
+      <c r="L81" t="n">
         <v>39982</v>
       </c>
-      <c r="L81" t="n">
+      <c r="M81" t="n">
+        <v>267029</v>
+      </c>
+      <c r="N81" t="n">
         <v>699.575</v>
-      </c>
-      <c r="M81" t="n">
-        <v>54</v>
-      </c>
-      <c r="N81" t="n">
-        <v>267029</v>
       </c>
       <c r="O81" t="n">
         <v>5840.575</v>
@@ -4876,16 +4876,16 @@
         <v>9.774999999999999</v>
       </c>
       <c r="K82" t="n">
+        <v>63.47499999999999</v>
+      </c>
+      <c r="L82" t="n">
         <v>29093.5</v>
       </c>
-      <c r="L82" t="n">
+      <c r="M82" t="n">
+        <v>265424.75</v>
+      </c>
+      <c r="N82" t="n">
         <v>900.625</v>
-      </c>
-      <c r="M82" t="n">
-        <v>63.47499999999999</v>
-      </c>
-      <c r="N82" t="n">
-        <v>265424.75</v>
       </c>
       <c r="O82" t="n">
         <v>6144.25</v>
@@ -4929,16 +4929,16 @@
         <v>24.075</v>
       </c>
       <c r="K83" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="L83" t="n">
         <v>20824.5</v>
       </c>
-      <c r="L83" t="n">
+      <c r="M83" t="n">
+        <v>258239.25</v>
+      </c>
+      <c r="N83" t="n">
         <v>631.65</v>
-      </c>
-      <c r="M83" t="n">
-        <v>82.59999999999999</v>
-      </c>
-      <c r="N83" t="n">
-        <v>258239.25</v>
       </c>
       <c r="O83" t="n">
         <v>5978.125</v>
@@ -4982,16 +4982,16 @@
         <v>0.3</v>
       </c>
       <c r="K84" t="n">
+        <v>55.72499999999999</v>
+      </c>
+      <c r="L84" t="n">
         <v>27006.25</v>
       </c>
-      <c r="L84" t="n">
+      <c r="M84" t="n">
+        <v>262936.75</v>
+      </c>
+      <c r="N84" t="n">
         <v>786</v>
-      </c>
-      <c r="M84" t="n">
-        <v>55.72499999999999</v>
-      </c>
-      <c r="N84" t="n">
-        <v>262936.75</v>
       </c>
       <c r="O84" t="n">
         <v>5943.549999999999</v>
@@ -5035,16 +5035,16 @@
         <v>0.3</v>
       </c>
       <c r="K85" t="n">
+        <v>43.375</v>
+      </c>
+      <c r="L85" t="n">
         <v>39477.75</v>
       </c>
-      <c r="L85" t="n">
+      <c r="M85" t="n">
+        <v>276732</v>
+      </c>
+      <c r="N85" t="n">
         <v>689.975</v>
-      </c>
-      <c r="M85" t="n">
-        <v>43.375</v>
-      </c>
-      <c r="N85" t="n">
-        <v>276732</v>
       </c>
       <c r="O85" t="n">
         <v>5770.375</v>
@@ -5088,16 +5088,16 @@
         <v>2.4</v>
       </c>
       <c r="K86" t="n">
+        <v>44.875</v>
+      </c>
+      <c r="L86" t="n">
         <v>24454.25</v>
       </c>
-      <c r="L86" t="n">
+      <c r="M86" t="n">
+        <v>271848.5</v>
+      </c>
+      <c r="N86" t="n">
         <v>674.025</v>
-      </c>
-      <c r="M86" t="n">
-        <v>44.875</v>
-      </c>
-      <c r="N86" t="n">
-        <v>271848.5</v>
       </c>
       <c r="O86" t="n">
         <v>5726.025</v>
@@ -5141,16 +5141,16 @@
         <v>0.3</v>
       </c>
       <c r="K87" t="n">
+        <v>38.25</v>
+      </c>
+      <c r="L87" t="n">
         <v>27241.5</v>
       </c>
-      <c r="L87" t="n">
+      <c r="M87" t="n">
+        <v>260605.75</v>
+      </c>
+      <c r="N87" t="n">
         <v>921.25</v>
-      </c>
-      <c r="M87" t="n">
-        <v>38.25</v>
-      </c>
-      <c r="N87" t="n">
-        <v>260605.75</v>
       </c>
       <c r="O87" t="n">
         <v>5958.299999999999</v>
@@ -5194,16 +5194,16 @@
         <v>0</v>
       </c>
       <c r="K88" t="n">
+        <v>37.15</v>
+      </c>
+      <c r="L88" t="n">
         <v>23022.5</v>
       </c>
-      <c r="L88" t="n">
+      <c r="M88" t="n">
+        <v>247545.75</v>
+      </c>
+      <c r="N88" t="n">
         <v>890.475</v>
-      </c>
-      <c r="M88" t="n">
-        <v>37.15</v>
-      </c>
-      <c r="N88" t="n">
-        <v>247545.75</v>
       </c>
       <c r="O88" t="n">
         <v>6193.575</v>
@@ -5247,16 +5247,16 @@
         <v>1.65</v>
       </c>
       <c r="K89" t="n">
+        <v>38.8</v>
+      </c>
+      <c r="L89" t="n">
         <v>30325.25</v>
       </c>
-      <c r="L89" t="n">
+      <c r="M89" t="n">
+        <v>243969.75</v>
+      </c>
+      <c r="N89" t="n">
         <v>945.475</v>
-      </c>
-      <c r="M89" t="n">
-        <v>38.8</v>
-      </c>
-      <c r="N89" t="n">
-        <v>243969.75</v>
       </c>
       <c r="O89" t="n">
         <v>6439.475</v>
@@ -5300,16 +5300,16 @@
         <v>1.3</v>
       </c>
       <c r="K90" t="n">
+        <v>40.1</v>
+      </c>
+      <c r="L90" t="n">
         <v>29065.5</v>
       </c>
-      <c r="L90" t="n">
+      <c r="M90" t="n">
+        <v>235278</v>
+      </c>
+      <c r="N90" t="n">
         <v>778.075</v>
-      </c>
-      <c r="M90" t="n">
-        <v>40.1</v>
-      </c>
-      <c r="N90" t="n">
-        <v>235278</v>
       </c>
       <c r="O90" t="n">
         <v>6316.925</v>
@@ -5353,16 +5353,16 @@
         <v>12.6</v>
       </c>
       <c r="K91" t="n">
+        <v>18.85</v>
+      </c>
+      <c r="L91" t="n">
         <v>21502.75</v>
       </c>
-      <c r="L91" t="n">
+      <c r="M91" t="n">
+        <v>233199.75</v>
+      </c>
+      <c r="N91" t="n">
         <v>743.975</v>
-      </c>
-      <c r="M91" t="n">
-        <v>18.85</v>
-      </c>
-      <c r="N91" t="n">
-        <v>233199.75</v>
       </c>
       <c r="O91" t="n">
         <v>6429.25</v>
@@ -5406,16 +5406,16 @@
         <v>0</v>
       </c>
       <c r="K92" t="n">
+        <v>18.85</v>
+      </c>
+      <c r="L92" t="n">
         <v>34715.5</v>
       </c>
-      <c r="L92" t="n">
+      <c r="M92" t="n">
+        <v>242974</v>
+      </c>
+      <c r="N92" t="n">
         <v>829.3</v>
-      </c>
-      <c r="M92" t="n">
-        <v>18.85</v>
-      </c>
-      <c r="N92" t="n">
-        <v>242974</v>
       </c>
       <c r="O92" t="n">
         <v>6472.549999999999</v>
@@ -5459,16 +5459,16 @@
         <v>24.125</v>
       </c>
       <c r="K93" t="n">
+        <v>42.675</v>
+      </c>
+      <c r="L93" t="n">
         <v>24953.75</v>
       </c>
-      <c r="L93" t="n">
+      <c r="M93" t="n">
+        <v>236116.75</v>
+      </c>
+      <c r="N93" t="n">
         <v>892.65</v>
-      </c>
-      <c r="M93" t="n">
-        <v>42.675</v>
-      </c>
-      <c r="N93" t="n">
-        <v>236116.75</v>
       </c>
       <c r="O93" t="n">
         <v>6675.225</v>
@@ -5512,16 +5512,16 @@
         <v>17.675</v>
       </c>
       <c r="K94" t="n">
+        <v>59.75</v>
+      </c>
+      <c r="L94" t="n">
         <v>19735.5</v>
       </c>
-      <c r="L94" t="n">
+      <c r="M94" t="n">
+        <v>223603.75</v>
+      </c>
+      <c r="N94" t="n">
         <v>895.575</v>
-      </c>
-      <c r="M94" t="n">
-        <v>59.75</v>
-      </c>
-      <c r="N94" t="n">
-        <v>223603.75</v>
       </c>
       <c r="O94" t="n">
         <v>6896.775000000001</v>
@@ -5565,16 +5565,16 @@
         <v>31</v>
       </c>
       <c r="K95" t="n">
+        <v>88.34999999999999</v>
+      </c>
+      <c r="L95" t="n">
         <v>20391</v>
       </c>
-      <c r="L95" t="n">
+      <c r="M95" t="n">
+        <v>217403.5</v>
+      </c>
+      <c r="N95" t="n">
         <v>827.1</v>
-      </c>
-      <c r="M95" t="n">
-        <v>88.34999999999999</v>
-      </c>
-      <c r="N95" t="n">
-        <v>217403.5</v>
       </c>
       <c r="O95" t="n">
         <v>6802.625</v>
@@ -5618,16 +5618,16 @@
         <v>42.1</v>
       </c>
       <c r="K96" t="n">
+        <v>130.45</v>
+      </c>
+      <c r="L96" t="n">
         <v>21469</v>
       </c>
-      <c r="L96" t="n">
+      <c r="M96" t="n">
+        <v>215560.25</v>
+      </c>
+      <c r="N96" t="n">
         <v>941.075</v>
-      </c>
-      <c r="M96" t="n">
-        <v>130.45</v>
-      </c>
-      <c r="N96" t="n">
-        <v>215560.25</v>
       </c>
       <c r="O96" t="n">
         <v>6853.225</v>
@@ -5671,16 +5671,16 @@
         <v>8.625</v>
       </c>
       <c r="K97" t="n">
+        <v>138.525</v>
+      </c>
+      <c r="L97" t="n">
         <v>24112.25</v>
       </c>
-      <c r="L97" t="n">
+      <c r="M97" t="n">
+        <v>215349.25</v>
+      </c>
+      <c r="N97" t="n">
         <v>880.025</v>
-      </c>
-      <c r="M97" t="n">
-        <v>138.525</v>
-      </c>
-      <c r="N97" t="n">
-        <v>215349.25</v>
       </c>
       <c r="O97" t="n">
         <v>6787.775</v>
@@ -5724,16 +5724,16 @@
         <v>4.2</v>
       </c>
       <c r="K98" t="n">
+        <v>141.625</v>
+      </c>
+      <c r="L98" t="n">
         <v>22754.25</v>
       </c>
-      <c r="L98" t="n">
+      <c r="M98" t="n">
+        <v>203391.25</v>
+      </c>
+      <c r="N98" t="n">
         <v>835.775</v>
-      </c>
-      <c r="M98" t="n">
-        <v>141.625</v>
-      </c>
-      <c r="N98" t="n">
-        <v>203391.25</v>
       </c>
       <c r="O98" t="n">
         <v>6845.475</v>
@@ -5777,16 +5777,16 @@
         <v>33.85</v>
       </c>
       <c r="K99" t="n">
+        <v>161.875</v>
+      </c>
+      <c r="L99" t="n">
         <v>21016.5</v>
       </c>
-      <c r="L99" t="n">
+      <c r="M99" t="n">
+        <v>202571.5</v>
+      </c>
+      <c r="N99" t="n">
         <v>789.125</v>
-      </c>
-      <c r="M99" t="n">
-        <v>161.875</v>
-      </c>
-      <c r="N99" t="n">
-        <v>202571.5</v>
       </c>
       <c r="O99" t="n">
         <v>6890.625</v>
@@ -5830,16 +5830,16 @@
         <v>16.85</v>
       </c>
       <c r="K100" t="n">
+        <v>178.425</v>
+      </c>
+      <c r="L100" t="n">
         <v>22731</v>
       </c>
-      <c r="L100" t="n">
+      <c r="M100" t="n">
+        <v>198492.5</v>
+      </c>
+      <c r="N100" t="n">
         <v>819.825</v>
-      </c>
-      <c r="M100" t="n">
-        <v>178.425</v>
-      </c>
-      <c r="N100" t="n">
-        <v>198492.5</v>
       </c>
       <c r="O100" t="n">
         <v>6881.150000000001</v>
@@ -5883,16 +5883,16 @@
         <v>23.4</v>
       </c>
       <c r="K101" t="n">
+        <v>201.825</v>
+      </c>
+      <c r="L101" t="n">
         <v>10742.5</v>
       </c>
-      <c r="L101" t="n">
+      <c r="M101" t="n">
+        <v>173718</v>
+      </c>
+      <c r="N101" t="n">
         <v>332.425</v>
-      </c>
-      <c r="M101" t="n">
-        <v>201.825</v>
-      </c>
-      <c r="N101" t="n">
-        <v>173718</v>
       </c>
       <c r="O101" t="n">
         <v>6320.925</v>
@@ -5936,16 +5936,16 @@
         <v>26.2</v>
       </c>
       <c r="K102" t="n">
+        <v>198.225</v>
+      </c>
+      <c r="L102" t="n">
         <v>17643.25</v>
       </c>
-      <c r="L102" t="n">
+      <c r="M102" t="n">
+        <v>170984</v>
+      </c>
+      <c r="N102" t="n">
         <v>600.025</v>
-      </c>
-      <c r="M102" t="n">
-        <v>198.225</v>
-      </c>
-      <c r="N102" t="n">
-        <v>170984</v>
       </c>
       <c r="O102" t="n">
         <v>6025.375</v>
@@ -5989,16 +5989,16 @@
         <v>5.325</v>
       </c>
       <c r="K103" t="n">
+        <v>178.7</v>
+      </c>
+      <c r="L103" t="n">
         <v>20303.25</v>
       </c>
-      <c r="L103" t="n">
+      <c r="M103" t="n">
+        <v>171337.75</v>
+      </c>
+      <c r="N103" t="n">
         <v>630.45</v>
-      </c>
-      <c r="M103" t="n">
-        <v>178.7</v>
-      </c>
-      <c r="N103" t="n">
-        <v>171337.75</v>
       </c>
       <c r="O103" t="n">
         <v>5828.724999999999</v>
@@ -6042,16 +6042,16 @@
         <v>15.35</v>
       </c>
       <c r="K104" t="n">
+        <v>174.3</v>
+      </c>
+      <c r="L104" t="n">
         <v>21240.5</v>
       </c>
-      <c r="L104" t="n">
+      <c r="M104" t="n">
+        <v>172034</v>
+      </c>
+      <c r="N104" t="n">
         <v>751.95</v>
-      </c>
-      <c r="M104" t="n">
-        <v>174.3</v>
-      </c>
-      <c r="N104" t="n">
-        <v>172034</v>
       </c>
       <c r="O104" t="n">
         <v>5639.6</v>
@@ -6095,16 +6095,16 @@
         <v>6.875</v>
       </c>
       <c r="K105" t="n">
+        <v>154.875</v>
+      </c>
+      <c r="L105" t="n">
         <v>8248.75</v>
       </c>
-      <c r="L105" t="n">
+      <c r="M105" t="n">
+        <v>175835.5</v>
+      </c>
+      <c r="N105" t="n">
         <v>204.6</v>
-      </c>
-      <c r="M105" t="n">
-        <v>154.875</v>
-      </c>
-      <c r="N105" t="n">
-        <v>175835.5</v>
       </c>
       <c r="O105" t="n">
         <v>4964.175</v>
@@ -6148,16 +6148,16 @@
         <v>0.3</v>
       </c>
       <c r="K106" t="n">
+        <v>132.35</v>
+      </c>
+      <c r="L106" t="n">
         <v>27384</v>
       </c>
-      <c r="L106" t="n">
+      <c r="M106" t="n">
+        <v>178857</v>
+      </c>
+      <c r="N106" t="n">
         <v>666.85</v>
-      </c>
-      <c r="M106" t="n">
-        <v>132.35</v>
-      </c>
-      <c r="N106" t="n">
-        <v>178857</v>
       </c>
       <c r="O106" t="n">
         <v>4795.25</v>
@@ -6201,16 +6201,16 @@
         <v>0.3</v>
       </c>
       <c r="K107" t="n">
+        <v>128.45</v>
+      </c>
+      <c r="L107" t="n">
         <v>21821.5</v>
       </c>
-      <c r="L107" t="n">
+      <c r="M107" t="n">
+        <v>175505</v>
+      </c>
+      <c r="N107" t="n">
         <v>579.25</v>
-      </c>
-      <c r="M107" t="n">
-        <v>128.45</v>
-      </c>
-      <c r="N107" t="n">
-        <v>175505</v>
       </c>
       <c r="O107" t="n">
         <v>4585.375</v>
@@ -6254,16 +6254,16 @@
         <v>0.3</v>
       </c>
       <c r="K108" t="n">
+        <v>94.89999999999999</v>
+      </c>
+      <c r="L108" t="n">
         <v>27870.75</v>
       </c>
-      <c r="L108" t="n">
+      <c r="M108" t="n">
+        <v>185839.75</v>
+      </c>
+      <c r="N108" t="n">
         <v>649.925</v>
-      </c>
-      <c r="M108" t="n">
-        <v>94.89999999999999</v>
-      </c>
-      <c r="N108" t="n">
-        <v>185839.75</v>
       </c>
       <c r="O108" t="n">
         <v>4415.475</v>
@@ -6307,16 +6307,16 @@
         <v>0</v>
       </c>
       <c r="K109" t="n">
+        <v>83.125</v>
+      </c>
+      <c r="L109" t="n">
         <v>28174</v>
       </c>
-      <c r="L109" t="n">
+      <c r="M109" t="n">
+        <v>189373.75</v>
+      </c>
+      <c r="N109" t="n">
         <v>822.775</v>
-      </c>
-      <c r="M109" t="n">
-        <v>83.125</v>
-      </c>
-      <c r="N109" t="n">
-        <v>189373.75</v>
       </c>
       <c r="O109" t="n">
         <v>4905.825</v>
@@ -6360,16 +6360,16 @@
         <v>2.2</v>
       </c>
       <c r="K110" t="n">
+        <v>66.55</v>
+      </c>
+      <c r="L110" t="n">
         <v>30220.75</v>
       </c>
-      <c r="L110" t="n">
+      <c r="M110" t="n">
+        <v>205844.25</v>
+      </c>
+      <c r="N110" t="n">
         <v>781.025</v>
-      </c>
-      <c r="M110" t="n">
-        <v>66.55</v>
-      </c>
-      <c r="N110" t="n">
-        <v>205844.25</v>
       </c>
       <c r="O110" t="n">
         <v>5086.825</v>
@@ -6413,16 +6413,16 @@
         <v>0.25</v>
       </c>
       <c r="K111" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="L111" t="n">
         <v>30376.5</v>
       </c>
-      <c r="L111" t="n">
+      <c r="M111" t="n">
+        <v>219091.75</v>
+      </c>
+      <c r="N111" t="n">
         <v>811.9</v>
-      </c>
-      <c r="M111" t="n">
-        <v>31.4</v>
-      </c>
-      <c r="N111" t="n">
-        <v>219091.75</v>
       </c>
       <c r="O111" t="n">
         <v>5268.275</v>
@@ -6466,16 +6466,16 @@
         <v>17.45</v>
       </c>
       <c r="K112" t="n">
+        <v>45.975</v>
+      </c>
+      <c r="L112" t="n">
         <v>24765.5</v>
       </c>
-      <c r="L112" t="n">
+      <c r="M112" t="n">
+        <v>228351.5</v>
+      </c>
+      <c r="N112" t="n">
         <v>607.025</v>
-      </c>
-      <c r="M112" t="n">
-        <v>45.975</v>
-      </c>
-      <c r="N112" t="n">
-        <v>228351.5</v>
       </c>
       <c r="O112" t="n">
         <v>5123.35</v>
@@ -6519,16 +6519,16 @@
         <v>21.5</v>
       </c>
       <c r="K113" t="n">
+        <v>49.175</v>
+      </c>
+      <c r="L113" t="n">
         <v>29114</v>
       </c>
-      <c r="L113" t="n">
+      <c r="M113" t="n">
+        <v>233790.75</v>
+      </c>
+      <c r="N113" t="n">
         <v>634.9</v>
-      </c>
-      <c r="M113" t="n">
-        <v>49.175</v>
-      </c>
-      <c r="N113" t="n">
-        <v>233790.75</v>
       </c>
       <c r="O113" t="n">
         <v>5553.65</v>
@@ -6572,16 +6572,16 @@
         <v>34.525</v>
       </c>
       <c r="K114" t="n">
+        <v>76.52499999999999</v>
+      </c>
+      <c r="L114" t="n">
         <v>27214</v>
       </c>
-      <c r="L114" t="n">
+      <c r="M114" t="n">
+        <v>235176</v>
+      </c>
+      <c r="N114" t="n">
         <v>682.875</v>
-      </c>
-      <c r="M114" t="n">
-        <v>76.52499999999999</v>
-      </c>
-      <c r="N114" t="n">
-        <v>235176</v>
       </c>
       <c r="O114" t="n">
         <v>5569.675</v>
@@ -6625,16 +6625,16 @@
         <v>7.6</v>
       </c>
       <c r="K115" t="n">
+        <v>84.12499999999999</v>
+      </c>
+      <c r="L115" t="n">
         <v>34572.5</v>
       </c>
-      <c r="L115" t="n">
+      <c r="M115" t="n">
+        <v>244599</v>
+      </c>
+      <c r="N115" t="n">
         <v>792.65</v>
-      </c>
-      <c r="M115" t="n">
-        <v>84.12499999999999</v>
-      </c>
-      <c r="N115" t="n">
-        <v>244599</v>
       </c>
       <c r="O115" t="n">
         <v>5783.075</v>
@@ -6678,16 +6678,16 @@
         <v>39.975</v>
       </c>
       <c r="K116" t="n">
+        <v>123.8</v>
+      </c>
+      <c r="L116" t="n">
         <v>28124.25</v>
       </c>
-      <c r="L116" t="n">
+      <c r="M116" t="n">
+        <v>249275.75</v>
+      </c>
+      <c r="N116" t="n">
         <v>782.875</v>
-      </c>
-      <c r="M116" t="n">
-        <v>123.8</v>
-      </c>
-      <c r="N116" t="n">
-        <v>249275.75</v>
       </c>
       <c r="O116" t="n">
         <v>5916.025</v>
@@ -6731,16 +6731,16 @@
         <v>18.075</v>
       </c>
       <c r="K117" t="n">
+        <v>141.575</v>
+      </c>
+      <c r="L117" t="n">
         <v>26944.25</v>
       </c>
-      <c r="L117" t="n">
+      <c r="M117" t="n">
+        <v>246998.25</v>
+      </c>
+      <c r="N117" t="n">
         <v>812.925</v>
-      </c>
-      <c r="M117" t="n">
-        <v>141.575</v>
-      </c>
-      <c r="N117" t="n">
-        <v>246998.25</v>
       </c>
       <c r="O117" t="n">
         <v>5906.175</v>
@@ -6784,16 +6784,16 @@
         <v>31.95</v>
       </c>
       <c r="K118" t="n">
+        <v>171.625</v>
+      </c>
+      <c r="L118" t="n">
         <v>23304.25</v>
       </c>
-      <c r="L118" t="n">
+      <c r="M118" t="n">
+        <v>242980.25</v>
+      </c>
+      <c r="N118" t="n">
         <v>696</v>
-      </c>
-      <c r="M118" t="n">
-        <v>171.625</v>
-      </c>
-      <c r="N118" t="n">
-        <v>242980.25</v>
       </c>
       <c r="O118" t="n">
         <v>5821.15</v>
@@ -6837,16 +6837,16 @@
         <v>22.25</v>
       </c>
       <c r="K119" t="n">
+        <v>193.575</v>
+      </c>
+      <c r="L119" t="n">
         <v>21133</v>
       </c>
-      <c r="L119" t="n">
+      <c r="M119" t="n">
+        <v>229848.5</v>
+      </c>
+      <c r="N119" t="n">
         <v>691.75</v>
-      </c>
-      <c r="M119" t="n">
-        <v>193.575</v>
-      </c>
-      <c r="N119" t="n">
-        <v>229848.5</v>
       </c>
       <c r="O119" t="n">
         <v>5701</v>
@@ -6890,16 +6890,16 @@
         <v>73.2</v>
       </c>
       <c r="K120" t="n">
+        <v>263.575</v>
+      </c>
+      <c r="L120" t="n">
         <v>23822.75</v>
       </c>
-      <c r="L120" t="n">
+      <c r="M120" t="n">
+        <v>226183</v>
+      </c>
+      <c r="N120" t="n">
         <v>697.05</v>
-      </c>
-      <c r="M120" t="n">
-        <v>263.575</v>
-      </c>
-      <c r="N120" t="n">
-        <v>226183</v>
       </c>
       <c r="O120" t="n">
         <v>5791.025000000001</v>
@@ -6943,16 +6943,16 @@
         <v>7.324999999999999</v>
       </c>
       <c r="K121" t="n">
+        <v>235.725</v>
+      </c>
+      <c r="L121" t="n">
         <v>25422.5</v>
       </c>
-      <c r="L121" t="n">
+      <c r="M121" t="n">
+        <v>228991.25</v>
+      </c>
+      <c r="N121" t="n">
         <v>560.725</v>
-      </c>
-      <c r="M121" t="n">
-        <v>235.725</v>
-      </c>
-      <c r="N121" t="n">
-        <v>228991.25</v>
       </c>
       <c r="O121" t="n">
         <v>5716.849999999999</v>
@@ -6996,16 +6996,16 @@
         <v>1.4</v>
       </c>
       <c r="K122" t="n">
+        <v>201.775</v>
+      </c>
+      <c r="L122" t="n">
         <v>33117</v>
       </c>
-      <c r="L122" t="n">
+      <c r="M122" t="n">
+        <v>232188</v>
+      </c>
+      <c r="N122" t="n">
         <v>768.575</v>
-      </c>
-      <c r="M122" t="n">
-        <v>201.775</v>
-      </c>
-      <c r="N122" t="n">
-        <v>232188</v>
       </c>
       <c r="O122" t="n">
         <v>5802.55</v>
@@ -7049,16 +7049,16 @@
         <v>0</v>
       </c>
       <c r="K123" t="n">
+        <v>195.525</v>
+      </c>
+      <c r="L123" t="n">
         <v>29712</v>
       </c>
-      <c r="L123" t="n">
+      <c r="M123" t="n">
+        <v>233028.5</v>
+      </c>
+      <c r="N123" t="n">
         <v>538.925</v>
-      </c>
-      <c r="M123" t="n">
-        <v>195.525</v>
-      </c>
-      <c r="N123" t="n">
-        <v>233028.5</v>
       </c>
       <c r="O123" t="n">
         <v>5548.825</v>
@@ -7102,16 +7102,16 @@
         <v>8.25</v>
       </c>
       <c r="K124" t="n">
+        <v>181.5</v>
+      </c>
+      <c r="L124" t="n">
         <v>25439.5</v>
       </c>
-      <c r="L124" t="n">
+      <c r="M124" t="n">
+        <v>225277</v>
+      </c>
+      <c r="N124" t="n">
         <v>578.825</v>
-      </c>
-      <c r="M124" t="n">
-        <v>181.5</v>
-      </c>
-      <c r="N124" t="n">
-        <v>225277</v>
       </c>
       <c r="O124" t="n">
         <v>5344.775000000001</v>
@@ -7155,16 +7155,16 @@
         <v>10.425</v>
       </c>
       <c r="K125" t="n">
+        <v>171.425</v>
+      </c>
+      <c r="L125" t="n">
         <v>26097</v>
       </c>
-      <c r="L125" t="n">
+      <c r="M125" t="n">
+        <v>224863</v>
+      </c>
+      <c r="N125" t="n">
         <v>744.8000000000001</v>
-      </c>
-      <c r="M125" t="n">
-        <v>171.425</v>
-      </c>
-      <c r="N125" t="n">
-        <v>224863</v>
       </c>
       <c r="O125" t="n">
         <v>5276.65</v>
@@ -7208,16 +7208,16 @@
         <v>13.3</v>
       </c>
       <c r="K126" t="n">
+        <v>152.9</v>
+      </c>
+      <c r="L126" t="n">
         <v>25619.75</v>
       </c>
-      <c r="L126" t="n">
+      <c r="M126" t="n">
+        <v>222317.5</v>
+      </c>
+      <c r="N126" t="n">
         <v>592.5500000000001</v>
-      </c>
-      <c r="M126" t="n">
-        <v>152.9</v>
-      </c>
-      <c r="N126" t="n">
-        <v>222317.5</v>
       </c>
       <c r="O126" t="n">
         <v>5173.2</v>
@@ -7261,16 +7261,16 @@
         <v>0</v>
       </c>
       <c r="K127" t="n">
+        <v>133.7</v>
+      </c>
+      <c r="L127" t="n">
         <v>31873.75</v>
       </c>
-      <c r="L127" t="n">
+      <c r="M127" t="n">
+        <v>233778.5</v>
+      </c>
+      <c r="N127" t="n">
         <v>689.775</v>
-      </c>
-      <c r="M127" t="n">
-        <v>133.7</v>
-      </c>
-      <c r="N127" t="n">
-        <v>233778.5</v>
       </c>
       <c r="O127" t="n">
         <v>5171.225</v>
@@ -7314,16 +7314,16 @@
         <v>0</v>
       </c>
       <c r="K128" t="n">
+        <v>75.77500000000001</v>
+      </c>
+      <c r="L128" t="n">
         <v>40493.25</v>
       </c>
-      <c r="L128" t="n">
+      <c r="M128" t="n">
+        <v>248792.75</v>
+      </c>
+      <c r="N128" t="n">
         <v>490.05</v>
-      </c>
-      <c r="M128" t="n">
-        <v>75.77500000000001</v>
-      </c>
-      <c r="N128" t="n">
-        <v>248792.75</v>
       </c>
       <c r="O128" t="n">
         <v>4964.225</v>
@@ -7367,16 +7367,16 @@
         <v>0</v>
       </c>
       <c r="K129" t="n">
+        <v>33.375</v>
+      </c>
+      <c r="L129" t="n">
         <v>32480.75</v>
       </c>
-      <c r="L129" t="n">
+      <c r="M129" t="n">
+        <v>257347</v>
+      </c>
+      <c r="N129" t="n">
         <v>466.6</v>
-      </c>
-      <c r="M129" t="n">
-        <v>33.375</v>
-      </c>
-      <c r="N129" t="n">
-        <v>257347</v>
       </c>
       <c r="O129" t="n">
         <v>4870.1</v>
@@ -7420,16 +7420,16 @@
         <v>0</v>
       </c>
       <c r="K130" t="n">
+        <v>32.275</v>
+      </c>
+      <c r="L130" t="n">
         <v>26572</v>
       </c>
-      <c r="L130" t="n">
+      <c r="M130" t="n">
+        <v>258656.75</v>
+      </c>
+      <c r="N130" t="n">
         <v>612.775</v>
-      </c>
-      <c r="M130" t="n">
-        <v>32.275</v>
-      </c>
-      <c r="N130" t="n">
-        <v>258656.75</v>
       </c>
       <c r="O130" t="n">
         <v>4714.299999999999</v>
@@ -7473,16 +7473,16 @@
         <v>27.625</v>
       </c>
       <c r="K131" t="n">
+        <v>59.6</v>
+      </c>
+      <c r="L131" t="n">
         <v>27070.75</v>
       </c>
-      <c r="L131" t="n">
+      <c r="M131" t="n">
+        <v>253534</v>
+      </c>
+      <c r="N131" t="n">
         <v>788.9</v>
-      </c>
-      <c r="M131" t="n">
-        <v>59.6</v>
-      </c>
-      <c r="N131" t="n">
-        <v>253534</v>
       </c>
       <c r="O131" t="n">
         <v>4964.275000000001</v>
@@ -7526,16 +7526,16 @@
         <v>45.575</v>
       </c>
       <c r="K132" t="n">
+        <v>105.175</v>
+      </c>
+      <c r="L132" t="n">
         <v>23897</v>
       </c>
-      <c r="L132" t="n">
+      <c r="M132" t="n">
+        <v>249354.25</v>
+      </c>
+      <c r="N132" t="n">
         <v>663.775</v>
-      </c>
-      <c r="M132" t="n">
-        <v>105.175</v>
-      </c>
-      <c r="N132" t="n">
-        <v>249354.25</v>
       </c>
       <c r="O132" t="n">
         <v>5049.224999999999</v>
@@ -7579,16 +7579,16 @@
         <v>17.05</v>
       </c>
       <c r="K133" t="n">
+        <v>113.975</v>
+      </c>
+      <c r="L133" t="n">
         <v>23714</v>
       </c>
-      <c r="L133" t="n">
+      <c r="M133" t="n">
+        <v>246527.75</v>
+      </c>
+      <c r="N133" t="n">
         <v>726.175</v>
-      </c>
-      <c r="M133" t="n">
-        <v>113.975</v>
-      </c>
-      <c r="N133" t="n">
-        <v>246527.75</v>
       </c>
       <c r="O133" t="n">
         <v>5030.599999999999</v>
@@ -7632,16 +7632,16 @@
         <v>0.3</v>
       </c>
       <c r="K134" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="L134" t="n">
         <v>26233.25</v>
       </c>
-      <c r="L134" t="n">
+      <c r="M134" t="n">
+        <v>244238.25</v>
+      </c>
+      <c r="N134" t="n">
         <v>855.875</v>
-      </c>
-      <c r="M134" t="n">
-        <v>99.7</v>
-      </c>
-      <c r="N134" t="n">
-        <v>244238.25</v>
       </c>
       <c r="O134" t="n">
         <v>5293.925</v>
@@ -7685,16 +7685,16 @@
         <v>34</v>
       </c>
       <c r="K135" t="n">
+        <v>124.55</v>
+      </c>
+      <c r="L135" t="n">
         <v>24122</v>
       </c>
-      <c r="L135" t="n">
+      <c r="M135" t="n">
+        <v>244811</v>
+      </c>
+      <c r="N135" t="n">
         <v>642.8</v>
-      </c>
-      <c r="M135" t="n">
-        <v>124.55</v>
-      </c>
-      <c r="N135" t="n">
-        <v>244811</v>
       </c>
       <c r="O135" t="n">
         <v>5246.95</v>
@@ -7738,16 +7738,16 @@
         <v>27.8</v>
       </c>
       <c r="K136" t="n">
+        <v>152.35</v>
+      </c>
+      <c r="L136" t="n">
         <v>26920.25</v>
       </c>
-      <c r="L136" t="n">
+      <c r="M136" t="n">
+        <v>234230.25</v>
+      </c>
+      <c r="N136" t="n">
         <v>722.375</v>
-      </c>
-      <c r="M136" t="n">
-        <v>152.35</v>
-      </c>
-      <c r="N136" t="n">
-        <v>234230.25</v>
       </c>
       <c r="O136" t="n">
         <v>5479.275</v>
@@ -7791,16 +7791,16 @@
         <v>20.425</v>
       </c>
       <c r="K137" t="n">
+        <v>172.775</v>
+      </c>
+      <c r="L137" t="n">
         <v>21929.5</v>
       </c>
-      <c r="L137" t="n">
+      <c r="M137" t="n">
+        <v>215063</v>
+      </c>
+      <c r="N137" t="n">
         <v>656.95</v>
-      </c>
-      <c r="M137" t="n">
-        <v>172.775</v>
-      </c>
-      <c r="N137" t="n">
-        <v>215063</v>
       </c>
       <c r="O137" t="n">
         <v>5669.625</v>
@@ -7844,16 +7844,16 @@
         <v>19.45</v>
       </c>
       <c r="K138" t="n">
+        <v>192.225</v>
+      </c>
+      <c r="L138" t="n">
         <v>30289.75</v>
       </c>
-      <c r="L138" t="n">
+      <c r="M138" t="n">
+        <v>219081.5</v>
+      </c>
+      <c r="N138" t="n">
         <v>692.225</v>
-      </c>
-      <c r="M138" t="n">
-        <v>192.225</v>
-      </c>
-      <c r="N138" t="n">
-        <v>219081.5</v>
       </c>
       <c r="O138" t="n">
         <v>5749.075000000001</v>
@@ -7897,16 +7897,16 @@
         <v>27.9</v>
       </c>
       <c r="K139" t="n">
+        <v>200.5</v>
+      </c>
+      <c r="L139" t="n">
         <v>23926.25</v>
       </c>
-      <c r="L139" t="n">
+      <c r="M139" t="n">
+        <v>216110</v>
+      </c>
+      <c r="N139" t="n">
         <v>737.675</v>
-      </c>
-      <c r="M139" t="n">
-        <v>200.5</v>
-      </c>
-      <c r="N139" t="n">
-        <v>216110</v>
       </c>
       <c r="O139" t="n">
         <v>5697.849999999999</v>
@@ -7950,16 +7950,16 @@
         <v>32</v>
       </c>
       <c r="K140" t="n">
+        <v>192.975</v>
+      </c>
+      <c r="L140" t="n">
         <v>27068</v>
       </c>
-      <c r="L140" t="n">
+      <c r="M140" t="n">
+        <v>219248.5</v>
+      </c>
+      <c r="N140" t="n">
         <v>689.925</v>
-      </c>
-      <c r="M140" t="n">
-        <v>192.975</v>
-      </c>
-      <c r="N140" t="n">
-        <v>219248.5</v>
       </c>
       <c r="O140" t="n">
         <v>5724</v>
@@ -8003,16 +8003,16 @@
         <v>3.075</v>
       </c>
       <c r="K141" t="n">
+        <v>173.7</v>
+      </c>
+      <c r="L141" t="n">
         <v>31153</v>
       </c>
-      <c r="L141" t="n">
+      <c r="M141" t="n">
+        <v>223721.5</v>
+      </c>
+      <c r="N141" t="n">
         <v>812.775</v>
-      </c>
-      <c r="M141" t="n">
-        <v>173.7</v>
-      </c>
-      <c r="N141" t="n">
-        <v>223721.5</v>
       </c>
       <c r="O141" t="n">
         <v>5810.6</v>
@@ -8056,16 +8056,16 @@
         <v>105.975</v>
       </c>
       <c r="K142" t="n">
+        <v>270.925</v>
+      </c>
+      <c r="L142" t="n">
         <v>24102.25</v>
       </c>
-      <c r="L142" t="n">
+      <c r="M142" t="n">
+        <v>226525.25</v>
+      </c>
+      <c r="N142" t="n">
         <v>720.475</v>
-      </c>
-      <c r="M142" t="n">
-        <v>270.925</v>
-      </c>
-      <c r="N142" t="n">
-        <v>226525.25</v>
       </c>
       <c r="O142" t="n">
         <v>5675.2</v>
@@ -8109,16 +8109,16 @@
         <v>29.075</v>
       </c>
       <c r="K143" t="n">
+        <v>296.275</v>
+      </c>
+      <c r="L143" t="n">
         <v>25555.75</v>
       </c>
-      <c r="L143" t="n">
+      <c r="M143" t="n">
+        <v>226109</v>
+      </c>
+      <c r="N143" t="n">
         <v>734.4</v>
-      </c>
-      <c r="M143" t="n">
-        <v>296.275</v>
-      </c>
-      <c r="N143" t="n">
-        <v>226109</v>
       </c>
       <c r="O143" t="n">
         <v>5766.799999999999</v>
@@ -8162,16 +8162,16 @@
         <v>16.75</v>
       </c>
       <c r="K144" t="n">
+        <v>262.2</v>
+      </c>
+      <c r="L144" t="n">
         <v>20723.75</v>
       </c>
-      <c r="L144" t="n">
+      <c r="M144" t="n">
+        <v>219515.25</v>
+      </c>
+      <c r="N144" t="n">
         <v>606.575</v>
-      </c>
-      <c r="M144" t="n">
-        <v>262.2</v>
-      </c>
-      <c r="N144" t="n">
-        <v>219515.25</v>
       </c>
       <c r="O144" t="n">
         <v>5651</v>
@@ -8215,16 +8215,16 @@
         <v>15.575</v>
       </c>
       <c r="K145" t="n">
+        <v>249.8</v>
+      </c>
+      <c r="L145" t="n">
         <v>19051.25</v>
       </c>
-      <c r="L145" t="n">
+      <c r="M145" t="n">
+        <v>214749</v>
+      </c>
+      <c r="N145" t="n">
         <v>718.025</v>
-      </c>
-      <c r="M145" t="n">
-        <v>249.8</v>
-      </c>
-      <c r="N145" t="n">
-        <v>214749</v>
       </c>
       <c r="O145" t="n">
         <v>5712.075</v>
@@ -8268,16 +8268,16 @@
         <v>16.775</v>
       </c>
       <c r="K146" t="n">
+        <v>266.275</v>
+      </c>
+      <c r="L146" t="n">
         <v>22078.25</v>
       </c>
-      <c r="L146" t="n">
+      <c r="M146" t="n">
+        <v>208770.5</v>
+      </c>
+      <c r="N146" t="n">
         <v>729.425</v>
-      </c>
-      <c r="M146" t="n">
-        <v>266.275</v>
-      </c>
-      <c r="N146" t="n">
-        <v>208770.5</v>
       </c>
       <c r="O146" t="n">
         <v>5749.275</v>
@@ -8321,16 +8321,16 @@
         <v>7.825</v>
       </c>
       <c r="K147" t="n">
+        <v>252.05</v>
+      </c>
+      <c r="L147" t="n">
         <v>21834.5</v>
       </c>
-      <c r="L147" t="n">
+      <c r="M147" t="n">
+        <v>207318.5</v>
+      </c>
+      <c r="N147" t="n">
         <v>716.35</v>
-      </c>
-      <c r="M147" t="n">
-        <v>252.05</v>
-      </c>
-      <c r="N147" t="n">
-        <v>207318.5</v>
       </c>
       <c r="O147" t="n">
         <v>5727.950000000001</v>
@@ -8374,16 +8374,16 @@
         <v>7.649999999999999</v>
       </c>
       <c r="K148" t="n">
+        <v>214.35</v>
+      </c>
+      <c r="L148" t="n">
         <v>22841</v>
       </c>
-      <c r="L148" t="n">
+      <c r="M148" t="n">
+        <v>205163.5</v>
+      </c>
+      <c r="N148" t="n">
         <v>636.625</v>
-      </c>
-      <c r="M148" t="n">
-        <v>214.35</v>
-      </c>
-      <c r="N148" t="n">
-        <v>205163.5</v>
       </c>
       <c r="O148" t="n">
         <v>5674.65</v>
@@ -8427,16 +8427,16 @@
         <v>35.7</v>
       </c>
       <c r="K149" t="n">
+        <v>238.4</v>
+      </c>
+      <c r="L149" t="n">
         <v>22903</v>
       </c>
-      <c r="L149" t="n">
+      <c r="M149" t="n">
+        <v>195518.5</v>
+      </c>
+      <c r="N149" t="n">
         <v>671.15</v>
-      </c>
-      <c r="M149" t="n">
-        <v>238.4</v>
-      </c>
-      <c r="N149" t="n">
-        <v>195518.5</v>
       </c>
       <c r="O149" t="n">
         <v>5533.025000000001</v>
@@ -8480,16 +8480,16 @@
         <v>14.35</v>
       </c>
       <c r="K150" t="n">
+        <v>218.15</v>
+      </c>
+      <c r="L150" t="n">
         <v>22888.25</v>
       </c>
-      <c r="L150" t="n">
+      <c r="M150" t="n">
+        <v>190213.75</v>
+      </c>
+      <c r="N150" t="n">
         <v>636.675</v>
-      </c>
-      <c r="M150" t="n">
-        <v>218.15</v>
-      </c>
-      <c r="N150" t="n">
-        <v>190213.75</v>
       </c>
       <c r="O150" t="n">
         <v>5449.225</v>
@@ -8533,16 +8533,16 @@
         <v>20</v>
       </c>
       <c r="K151" t="n">
+        <v>157.35</v>
+      </c>
+      <c r="L151" t="n">
         <v>23914.25</v>
       </c>
-      <c r="L151" t="n">
+      <c r="M151" t="n">
+        <v>189959.25</v>
+      </c>
+      <c r="N151" t="n">
         <v>644.525</v>
-      </c>
-      <c r="M151" t="n">
-        <v>157.35</v>
-      </c>
-      <c r="N151" t="n">
-        <v>189959.25</v>
       </c>
       <c r="O151" t="n">
         <v>5359.35</v>
@@ -8586,16 +8586,16 @@
         <v>10.95</v>
       </c>
       <c r="K152" t="n">
+        <v>140.55</v>
+      </c>
+      <c r="L152" t="n">
         <v>20219.25</v>
       </c>
-      <c r="L152" t="n">
+      <c r="M152" t="n">
+        <v>188156</v>
+      </c>
+      <c r="N152" t="n">
         <v>527.675</v>
-      </c>
-      <c r="M152" t="n">
-        <v>140.55</v>
-      </c>
-      <c r="N152" t="n">
-        <v>188156</v>
       </c>
       <c r="O152" t="n">
         <v>5280.45</v>
@@ -8639,16 +8639,16 @@
         <v>13.175</v>
       </c>
       <c r="K153" t="n">
+        <v>142</v>
+      </c>
+      <c r="L153" t="n">
         <v>22702.75</v>
       </c>
-      <c r="L153" t="n">
+      <c r="M153" t="n">
+        <v>190086.25</v>
+      </c>
+      <c r="N153" t="n">
         <v>581</v>
-      </c>
-      <c r="M153" t="n">
-        <v>142</v>
-      </c>
-      <c r="N153" t="n">
-        <v>190086.25</v>
       </c>
       <c r="O153" t="n">
         <v>5143.425</v>
@@ -8692,16 +8692,16 @@
         <v>2.225</v>
       </c>
       <c r="K154" t="n">
+        <v>115.575</v>
+      </c>
+      <c r="L154" t="n">
         <v>22733.5</v>
       </c>
-      <c r="L154" t="n">
+      <c r="M154" t="n">
+        <v>192217.25</v>
+      </c>
+      <c r="N154" t="n">
         <v>571.85</v>
-      </c>
-      <c r="M154" t="n">
-        <v>115.575</v>
-      </c>
-      <c r="N154" t="n">
-        <v>192217.25</v>
       </c>
       <c r="O154" t="n">
         <v>4985.849999999999</v>
@@ -8745,16 +8745,16 @@
         <v>2.75</v>
       </c>
       <c r="K155" t="n">
+        <v>115.65</v>
+      </c>
+      <c r="L155" t="n">
         <v>3191.25</v>
       </c>
-      <c r="L155" t="n">
+      <c r="M155" t="n">
+        <v>193078.25</v>
+      </c>
+      <c r="N155" t="n">
         <v>96</v>
-      </c>
-      <c r="M155" t="n">
-        <v>115.65</v>
-      </c>
-      <c r="N155" t="n">
-        <v>193078.25</v>
       </c>
       <c r="O155" t="n">
         <v>4365.5</v>
@@ -8920,7 +8920,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Radiación estimada (Wh/m²)</t>
+          <t>Precipitación estimada acumulada últimos 60 días (mm)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -8932,7 +8932,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Grados-día calefacción (HDD)</t>
+          <t>Radiación estimada (Wh/m²)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -8944,7 +8944,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Precipitación estimada acumulada últimos 60 días (mm)</t>
+          <t>Radiación estimada acumulada últimos 60 días (Wh/m²)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -8956,7 +8956,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Radiación estimada acumulada últimos 60 días (Wh/m²)</t>
+          <t>Grados-día calefacción (HDD)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">

</xml_diff>

<commit_message>
fix: se corrije el orden de panel de descripcion
</commit_message>
<xml_diff>
--- a/resumen_semanal_clima.xlsx
+++ b/resumen_semanal_clima.xlsx
@@ -8925,7 +8925,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Total semanal estimado de energía solar recibida en Wh/m²</t>
+          <t>Acumulado de precipitación estimada en los 60 días anteriores</t>
         </is>
       </c>
     </row>
@@ -8937,7 +8937,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Total semanal de Heating Degree DaysGrados-día de calefacción: suma de (T_base - T) * 0.25 cada 15 minutos</t>
+          <t>Total semanal estimado de energía solar recibida en Wh/m²</t>
         </is>
       </c>
     </row>
@@ -8949,7 +8949,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Acumulado de precipitación estimada en los 60 días anteriores</t>
+          <t>Acumulado de radiación estimada en los 60 días anteriores</t>
         </is>
       </c>
     </row>
@@ -8961,7 +8961,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Acumulado de radiación estimada en los 60 días anteriores</t>
+          <t>Total semanal de Heating Degree DaysGrados-día de calefacción: suma de (T_base - T) * 0.25 cada 15 minutos</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: se agregan los graficos para los cumulados de 60 dias
</commit_message>
<xml_diff>
--- a/resumen_semanal_clima.xlsx
+++ b/resumen_semanal_clima.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Resumen semanal" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Descripción" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Gráficos" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Acumulados 60d" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -143,6 +144,86 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="11430000" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>29</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="11430000" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>58</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="11430000" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -9023,4 +9104,23 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>